<commit_message>
Union of Two Array.cpp
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C12911-E9A5-44DF-8E3A-F2C24582D004}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B232D3-0C47-4090-9A6E-3CBCD8611B43}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1913,7 +1913,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2029,7 +2029,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="21">
-      <c r="A11">
+      <c r="A11" s="12">
         <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2038,8 +2038,8 @@
       <c r="C11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>4</v>
+      <c r="D11" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Minimize the heights added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3187775F-FCD1-4F29-BD4E-1953EB00AE0D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC393001-DB6F-4FD3-9ED9-20184ADB0498}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1913,7 +1913,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2071,7 +2071,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="21">
-      <c r="A14">
+      <c r="A14" s="12">
         <v>9</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -2080,8 +2080,8 @@
       <c r="C14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>4</v>
+      <c r="D14" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="21">

</xml_diff>

<commit_message>
DP Soln of Min Jumps added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC393001-DB6F-4FD3-9ED9-20184ADB0498}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7D3EB3-9A7F-4CDB-BB5C-202C26BFF86B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>

</xml_diff>

<commit_message>
O(n) Solution of Max Jumps added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7D3EB3-9A7F-4CDB-BB5C-202C26BFF86B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13208255-577A-4629-8FD5-4BED7FFE0178}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1556,7 +1556,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1590,6 +1590,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1912,8 +1913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1924,7 +1925,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24.6">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>466</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1932,14 +1933,14 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="15"/>
+      <c r="A2" s="16"/>
       <c r="C2" s="8" t="s">
         <v>464</v>
       </c>
       <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="15"/>
+      <c r="A3" s="16"/>
       <c r="D3" s="12"/>
     </row>
     <row r="4" spans="1:4" ht="21">
@@ -2071,7 +2072,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="21">
-      <c r="A14" s="12">
+      <c r="A14" s="15">
         <v>9</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -2085,7 +2086,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="21">
-      <c r="A15">
+      <c r="A15" s="15">
         <v>10</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -2094,8 +2095,8 @@
       <c r="C15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>4</v>
+      <c r="D15" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Merge without extra Space prg added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30005CB9-6A91-47BE-93D6-C48188A3CC56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FC50E0-28CE-4D98-9A31-50E1692F12FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1913,7 +1913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Next Permutation problem added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F00C4C8-E8BF-4307-BE22-D49BB7951651}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06F307E-34E5-441E-AC22-A645DA793A31}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="468">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1426,6 +1426,9 @@
   </si>
   <si>
     <t>find duplicate in an array of N+1 Integers (New Algo  Learnt : Floyd's Algo)</t>
+  </si>
+  <si>
+    <t>Yellow Means new concept learned and needs to be revised</t>
   </si>
 </sst>
 </file>
@@ -1913,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1955,6 +1958,10 @@
       </c>
     </row>
     <row r="5" spans="1:4">
+      <c r="B5" s="15"/>
+      <c r="C5" t="s">
+        <v>467</v>
+      </c>
       <c r="D5" s="14" t="s">
         <v>4</v>
       </c>
@@ -2156,7 +2163,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="21">
-      <c r="A20">
+      <c r="A20" s="15">
         <v>15</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -2165,8 +2172,8 @@
       <c r="C20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="10" t="s">
-        <v>4</v>
+      <c r="D20" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Best time to buy and Count Pairs of Sum added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFE6207-C3A6-4DF5-A656-B5B1E3541F96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112578BC-6621-4F0A-9A84-881B69F62DFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1916,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="77" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1925,6 +1925,7 @@
     <col min="2" max="2" width="28.5" customWidth="1"/>
     <col min="3" max="3" width="123" customWidth="1"/>
     <col min="4" max="4" width="27.5" style="9" customWidth="1"/>
+    <col min="5" max="5" width="23.09765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24.6">
@@ -2191,7 +2192,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="21">
-      <c r="A22">
+      <c r="A22" s="12">
         <v>17</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -2200,12 +2201,12 @@
       <c r="C22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="10" t="s">
-        <v>4</v>
+      <c r="D22" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="21">
-      <c r="A23">
+      <c r="A23" s="12">
         <v>18</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -2214,8 +2215,8 @@
       <c r="C23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="10" t="s">
-        <v>4</v>
+      <c r="D23" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Common elements in 3 sorted array added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112578BC-6621-4F0A-9A84-881B69F62DFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB49D2B-7546-47EC-ADD2-A4FD2B706036}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1916,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="77" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="77" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2220,7 +2220,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="21">
-      <c r="A24">
+      <c r="A24" s="12">
         <v>19</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -2229,8 +2229,8 @@
       <c r="C24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="10" t="s">
-        <v>4</v>
+      <c r="D24" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Rearrange Array in Elements
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB49D2B-7546-47EC-ADD2-A4FD2B706036}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6818C13B-CAFE-41B3-85D0-31130346CAEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1916,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="77" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E27" sqref="E26:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2234,7 +2234,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="21">
-      <c r="A25">
+      <c r="A25" s="12">
         <v>20</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -2243,8 +2243,8 @@
       <c r="C25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>4</v>
+      <c r="D25" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Subarray Sum Zero added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6818C13B-CAFE-41B3-85D0-31130346CAEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECF1370-CF95-4D10-A2F5-0BFDD5485EB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1916,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E27" sqref="E26:E27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2248,7 +2248,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="21">
-      <c r="A26">
+      <c r="A26" s="12">
         <v>21</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -2257,8 +2257,8 @@
       <c r="C26" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="10" t="s">
-        <v>4</v>
+      <c r="D26" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Factorial of large number added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECF1370-CF95-4D10-A2F5-0BFDD5485EB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941D2BC9-5BC3-44F3-BDF9-B2DD3068147C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1916,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2262,7 +2262,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="21">
-      <c r="A27">
+      <c r="A27" s="12">
         <v>22</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -2271,8 +2271,8 @@
       <c r="C27" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>4</v>
+      <c r="D27" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Max Product Subarray added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941D2BC9-5BC3-44F3-BDF9-B2DD3068147C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9061699B-3122-4706-8F9D-4BB0C7168754}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1916,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2276,7 +2276,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="21">
-      <c r="A28">
+      <c r="A28" s="15">
         <v>23</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -2285,8 +2285,8 @@
       <c r="C28" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>4</v>
+      <c r="D28" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="21">

</xml_diff>

<commit_message>
LongConsSeq and NdK elemments problem added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9061699B-3122-4706-8F9D-4BB0C7168754}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E2F935-370D-4A75-9472-ACBEA5E96518}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1916,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2290,7 +2290,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="21">
-      <c r="A29">
+      <c r="A29" s="12">
         <v>24</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -2299,12 +2299,12 @@
       <c r="C29" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="10" t="s">
-        <v>4</v>
+      <c r="D29" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="21">
-      <c r="A30">
+      <c r="A30" s="15">
         <v>25</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -2313,8 +2313,8 @@
       <c r="C30" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="10" t="s">
-        <v>4</v>
+      <c r="D30" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Buy and Sell stocks at most two times
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E2F935-370D-4A75-9472-ACBEA5E96518}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F08BC41-DCF9-47A5-B4E3-693B75F240FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1916,12 +1916,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="28.5" customWidth="1"/>
     <col min="3" max="3" width="123" customWidth="1"/>
     <col min="4" max="4" width="27.5" style="9" customWidth="1"/>
@@ -2318,7 +2319,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="21">
-      <c r="A31">
+      <c r="A31" s="15">
         <v>26</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -2327,8 +2328,8 @@
       <c r="C31" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="10" t="s">
-        <v>4</v>
+      <c r="D31" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Array is A Subset of another Array
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F08BC41-DCF9-47A5-B4E3-693B75F240FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61EA9D3-2D09-4A63-AB4D-0F7D49A21B50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1917,7 +1917,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2333,7 +2333,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="21">
-      <c r="A32">
+      <c r="A32" s="12">
         <v>27</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -2342,8 +2342,8 @@
       <c r="C32" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="10" t="s">
-        <v>4</v>
+      <c r="D32" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Triplet Sum in Array added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61EA9D3-2D09-4A63-AB4D-0F7D49A21B50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAECD7E3-43AB-4C2A-9519-6EE08529CD1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1916,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2347,7 +2347,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="21">
-      <c r="A33">
+      <c r="A33" s="12">
         <v>28</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -2356,8 +2356,8 @@
       <c r="C33" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="10" t="s">
-        <v>4</v>
+      <c r="D33" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Trapping Rain Water added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAECD7E3-43AB-4C2A-9519-6EE08529CD1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB490858-E1EC-4FE4-BD64-000021D52E23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1595,7 +1595,7 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1916,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="83" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1949,6 +1949,7 @@
       <c r="D3" s="12"/>
     </row>
     <row r="4" spans="1:4" ht="21">
+      <c r="A4" s="16"/>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -2361,7 +2362,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="21">
-      <c r="A34">
+      <c r="A34" s="15">
         <v>29</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -2370,8 +2371,8 @@
       <c r="C34" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="10" t="s">
-        <v>4</v>
+      <c r="D34" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="21">
@@ -8348,7 +8349,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A1:A4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Chocolate Distribution Problem added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB490858-E1EC-4FE4-BD64-000021D52E23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731CB571-406F-4D4B-8AF8-4C08A5B59EE2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1916,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="83" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="83" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2376,7 +2376,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="21">
-      <c r="A35">
+      <c r="A35" s="12">
         <v>30</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -2385,8 +2385,8 @@
       <c r="C35" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="10" t="s">
-        <v>4</v>
+      <c r="D35" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Smallest Subarray with Sum added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731CB571-406F-4D4B-8AF8-4C08A5B59EE2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9730D6-46CD-4312-8BA6-36C65E25E362}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1917,7 +1917,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" zoomScale="83" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2390,7 +2390,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="21">
-      <c r="A36">
+      <c r="A36" s="12">
         <v>31</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -2399,8 +2399,8 @@
       <c r="C36" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="10" t="s">
-        <v>4</v>
+      <c r="D36" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Three Way Partitioning of Array added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9730D6-46CD-4312-8BA6-36C65E25E362}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18EB73D-611F-45A6-AA5E-4F9F63C83A36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1917,7 +1917,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" zoomScale="83" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2404,7 +2404,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="21">
-      <c r="A37">
+      <c r="A37" s="12">
         <v>32</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -2413,8 +2413,8 @@
       <c r="C37" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="10" t="s">
-        <v>4</v>
+      <c r="D37" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Palindrome array and Minimum Swaps added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18EB73D-611F-45A6-AA5E-4F9F63C83A36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D819162D-F836-4B96-9D06-C61D9C066527}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1917,7 +1917,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" zoomScale="83" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2418,7 +2418,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="21">
-      <c r="A38">
+      <c r="A38" s="15">
         <v>33</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -2427,12 +2427,12 @@
       <c r="C38" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="10" t="s">
-        <v>4</v>
+      <c r="D38" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="21">
-      <c r="A39">
+      <c r="A39" s="12">
         <v>34</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -2441,8 +2441,8 @@
       <c r="C39" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="10" t="s">
-        <v>4</v>
+      <c r="D39" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Spiral Traversal of Matrix added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52495140-11D6-4644-90EC-D168273B8EDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDF0DAC-97A2-442A-9A38-E26FA817F5B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="469">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1429,6 +1429,9 @@
   </si>
   <si>
     <t>Median of 2 sorted arrays of different size   Excellent Question…. Must Read</t>
+  </si>
+  <si>
+    <t>Just Read the Stuff. Highly Intuitive. Must Revise</t>
   </si>
 </sst>
 </file>
@@ -1916,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="83" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="83" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1925,7 +1928,7 @@
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="28.5" customWidth="1"/>
     <col min="3" max="3" width="123" customWidth="1"/>
-    <col min="4" max="4" width="27.5" style="9" customWidth="1"/>
+    <col min="4" max="4" width="42.3984375" style="9" customWidth="1"/>
     <col min="5" max="5" width="23.09765625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2469,25 +2472,21 @@
       <c r="C41" s="4" t="s">
         <v>467</v>
       </c>
-      <c r="D41" s="10" t="s">
-        <v>4</v>
+      <c r="D41" s="11" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="21">
       <c r="C42" s="5"/>
-      <c r="D42" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="D42"/>
     </row>
     <row r="43" spans="1:4" ht="21">
       <c r="B43" s="3"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="D43"/>
     </row>
     <row r="44" spans="1:4" ht="21">
-      <c r="A44">
+      <c r="A44" s="15">
         <v>37</v>
       </c>
       <c r="B44" s="6" t="s">
@@ -2496,8 +2495,8 @@
       <c r="C44" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="10" t="s">
-        <v>4</v>
+      <c r="D44" s="11" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Row with max 1s added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251704BE-839F-4EA9-946D-640A2A3196C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD0BF79-9AB7-4627-A936-0ACD2C10B95E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1919,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="83" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="83" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2528,7 +2528,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="21">
-      <c r="A47">
+      <c r="A47" s="15">
         <v>40</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -2537,8 +2537,8 @@
       <c r="C47" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D47" s="10" t="s">
-        <v>4</v>
+      <c r="D47" s="11" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Kth smallest element in matrix added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B24A932-5CDD-4660-9435-4899A602AF17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818B6530-9BCF-4D29-BDB2-8421600214AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1919,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="83" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="B39" zoomScale="83" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2598,7 +2598,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="21">
-      <c r="A52">
+      <c r="A52" s="12">
         <v>45</v>
       </c>
       <c r="B52" s="6" t="s">
@@ -2607,8 +2607,8 @@
       <c r="C52" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D52" s="10" t="s">
-        <v>4</v>
+      <c r="D52" s="11" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Common elements in all row added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818B6530-9BCF-4D29-BDB2-8421600214AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA7AB6E-C8EB-420B-BA4E-394E6271237C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1919,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B39" zoomScale="83" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="83" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2612,7 +2612,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="21">
-      <c r="A53">
+      <c r="A53" s="12">
         <v>46</v>
       </c>
       <c r="B53" s="6" t="s">
@@ -2621,8 +2621,8 @@
       <c r="C53" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D53" s="10" t="s">
-        <v>4</v>
+      <c r="D53" s="11" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Reverse a String added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC670D39-E462-4297-AB51-8D4263F9A7A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C81ABB-A006-4227-9139-DF7D2A83FD03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1919,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="83" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="84" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2625,13 +2625,16 @@
         <v>460</v>
       </c>
     </row>
+    <row r="54" spans="1:4">
+      <c r="D54"/>
+    </row>
     <row r="55" spans="1:4" ht="21">
       <c r="B55" s="3"/>
       <c r="C55" s="5"/>
-      <c r="D55" s="10"/>
+      <c r="D55"/>
     </row>
     <row r="56" spans="1:4" ht="21">
-      <c r="A56">
+      <c r="A56" s="12">
         <v>47</v>
       </c>
       <c r="B56" s="3" t="s">
@@ -2640,8 +2643,8 @@
       <c r="C56" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D56" s="10" t="s">
-        <v>4</v>
+      <c r="D56" s="11" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Palindrome String check added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C81ABB-A006-4227-9139-DF7D2A83FD03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961036FF-AD96-43E3-8D76-9642033F1957}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1919,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="84" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="84" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2648,7 +2648,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="21">
-      <c r="A57">
+      <c r="A57" s="12">
         <v>48</v>
       </c>
       <c r="B57" s="3" t="s">
@@ -2657,8 +2657,8 @@
       <c r="C57" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D57" s="10" t="s">
-        <v>4</v>
+      <c r="D57" s="11" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Shuffle Checking two strings added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97196576-F401-4D8F-A396-17315F95EE81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552BFEE9-204D-4DE2-BA17-7E9386A8AB7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1919,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="78" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="78" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2704,7 +2704,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="21">
-      <c r="A61">
+      <c r="A61" s="12">
         <v>52</v>
       </c>
       <c r="B61" s="3" t="s">
@@ -2713,8 +2713,8 @@
       <c r="C61" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D61" s="10" t="s">
-        <v>4</v>
+      <c r="D61" s="11" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Count and Say problem added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552BFEE9-204D-4DE2-BA17-7E9386A8AB7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0FF898-D92F-4DE4-87D9-C0C539C94C99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1919,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="78" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="78" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2718,7 +2718,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="21">
-      <c r="A62">
+      <c r="A62" s="12">
         <v>53</v>
       </c>
       <c r="B62" s="3" t="s">
@@ -2727,8 +2727,8 @@
       <c r="C62" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D62" s="10" t="s">
-        <v>4</v>
+      <c r="D62" s="11" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Longest  Subsequence of string
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA77F502-1C94-4AE6-B270-3A22DD2F714A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3DCCA2-B578-4ECE-81A1-D97247DA3401}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1919,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="78" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="78" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3054,7 +3054,7 @@
       </c>
     </row>
     <row r="86" spans="1:4" ht="21">
-      <c r="A86">
+      <c r="A86" s="15">
         <v>77</v>
       </c>
       <c r="B86" s="3" t="s">
@@ -3063,8 +3063,8 @@
       <c r="C86" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D86" s="10" t="s">
-        <v>4</v>
+      <c r="D86" s="11" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Print all Subsequences of String added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3DCCA2-B578-4ECE-81A1-D97247DA3401}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D2441C-2081-4BD2-A3DF-985FA96BAA04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1919,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="78" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView tabSelected="1" topLeftCell="C51" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2746,7 +2746,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="21">
-      <c r="A64">
+      <c r="A64" s="15">
         <v>55</v>
       </c>
       <c r="B64" s="3" t="s">
@@ -2755,12 +2755,12 @@
       <c r="C64" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D64" s="10" t="s">
-        <v>4</v>
+      <c r="D64" s="11" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="21">
-      <c r="A65">
+      <c r="A65" s="12">
         <v>56</v>
       </c>
       <c r="B65" s="3" t="s">
@@ -2769,8 +2769,8 @@
       <c r="C65" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D65" s="10" t="s">
-        <v>4</v>
+      <c r="D65" s="11" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Permutations of String added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D2441C-2081-4BD2-A3DF-985FA96BAA04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582153D0-B898-4492-B2AB-6FD9255B42EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1919,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C51" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2774,7 +2774,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="21">
-      <c r="A66">
+      <c r="A66" s="15">
         <v>57</v>
       </c>
       <c r="B66" s="3" t="s">
@@ -2783,8 +2783,8 @@
       <c r="C66" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D66" s="10" t="s">
-        <v>4</v>
+      <c r="D66" s="11" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Equivalent Mobile Number added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E363951-7FB0-41F8-9080-9D51D5BE0448}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C44BCA7-2FAB-4109-82CE-03229FD579D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1919,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B60" zoomScale="79" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2900,7 +2900,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="21">
-      <c r="A75">
+      <c r="A75" s="12">
         <v>66</v>
       </c>
       <c r="B75" s="3" t="s">
@@ -2909,8 +2909,8 @@
       <c r="C75" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D75" s="10" t="s">
-        <v>4</v>
+      <c r="D75" s="11" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Count the reversals added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C44BCA7-2FAB-4109-82CE-03229FD579D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E46ADF-2854-46C2-A4E7-77322B29B703}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1920,7 +1920,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2914,7 +2914,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="21">
-      <c r="A76">
+      <c r="A76" s="12">
         <v>67</v>
       </c>
       <c r="B76" s="3" t="s">
@@ -2923,8 +2923,8 @@
       <c r="C76" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D76" s="10" t="s">
-        <v>4</v>
+      <c r="D76" s="11" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Count all palindrome subsequences added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E46ADF-2854-46C2-A4E7-77322B29B703}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9F9C84-36AB-47C8-9F0A-6EE0E3B75C9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1919,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2937,8 +2937,8 @@
       <c r="C77" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D77" s="10" t="s">
-        <v>4</v>
+      <c r="D77" s="11" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Count of no of String in 2d char matrix
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB9D88E-1748-4D2D-BD64-6130BC1E44F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0374C58-01F0-49C4-BD92-744CB13A4ACC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1920,7 +1920,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A68" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2942,7 +2942,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" ht="21">
-      <c r="A78">
+      <c r="A78" s="12">
         <v>69</v>
       </c>
       <c r="B78" s="3" t="s">
@@ -2951,8 +2951,8 @@
       <c r="C78" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D78" s="10" t="s">
-        <v>4</v>
+      <c r="D78" s="11" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Search a Word in 2D Grid added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0374C58-01F0-49C4-BD92-744CB13A4ACC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED35007-5E16-4935-A921-09626E9D5C68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1920,7 +1920,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A68" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2956,7 +2956,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" ht="21">
-      <c r="A79">
+      <c r="A79" s="15">
         <v>70</v>
       </c>
       <c r="B79" s="3" t="s">
@@ -2965,8 +2965,8 @@
       <c r="C79" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D79" s="10" t="s">
-        <v>4</v>
+      <c r="D79" s="11" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Longest Common Prefix added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED35007-5E16-4935-A921-09626E9D5C68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5599E9BF-846E-4820-9769-842E060ADEBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1919,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2970,7 +2970,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="21">
-      <c r="A80">
+      <c r="A80" s="15">
         <v>71</v>
       </c>
       <c r="B80" s="3" t="s">
@@ -2984,7 +2984,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" ht="21">
-      <c r="A81">
+      <c r="A81" s="12">
         <v>72</v>
       </c>
       <c r="B81" s="3" t="s">
@@ -2993,12 +2993,12 @@
       <c r="C81" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D81" s="10" t="s">
-        <v>4</v>
+      <c r="D81" s="11" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="21">
-      <c r="A82">
+      <c r="A82" s="12">
         <v>73</v>
       </c>
       <c r="B82" s="3" t="s">
@@ -3007,8 +3007,8 @@
       <c r="C82" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D82" s="10" t="s">
-        <v>4</v>
+      <c r="D82" s="11" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Number of flips to make binary string alternate
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5599E9BF-846E-4820-9769-842E060ADEBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB43A588-2F15-4ECF-9076-9C7784A84D42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1920,7 +1920,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3012,7 +3012,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" ht="21">
-      <c r="A83">
+      <c r="A83" s="15">
         <v>74</v>
       </c>
       <c r="B83" s="3" t="s">
@@ -3021,8 +3021,8 @@
       <c r="C83" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D83" s="10" t="s">
-        <v>4</v>
+      <c r="D83" s="11" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="21">

</xml_diff>

<commit_message>
First Repeated Word in a String added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB43A588-2F15-4ECF-9076-9C7784A84D42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C712E3-3374-4672-90DA-0CA689EBE583}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1920,7 +1920,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3026,7 +3026,7 @@
       </c>
     </row>
     <row r="84" spans="1:4" ht="21">
-      <c r="A84">
+      <c r="A84" s="12">
         <v>75</v>
       </c>
       <c r="B84" s="3" t="s">
@@ -3035,8 +3035,8 @@
       <c r="C84" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D84" s="10" t="s">
-        <v>4</v>
+      <c r="D84" s="11" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Added problems 76,78 and 79.
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C712E3-3374-4672-90DA-0CA689EBE583}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BF358E-8660-487D-B01D-A7DC42B1C713}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1523,7 +1523,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1546,6 +1546,12 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1562,7 +1568,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1600,6 +1606,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -1919,8 +1926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3040,7 +3047,7 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="21">
-      <c r="A85">
+      <c r="A85" s="15">
         <v>76</v>
       </c>
       <c r="B85" s="3" t="s">
@@ -3068,7 +3075,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" ht="21">
-      <c r="A87">
+      <c r="A87" s="17">
         <v>78</v>
       </c>
       <c r="B87" s="3" t="s">

</xml_diff>

<commit_message>
Smallest Distinct window O(n2) soln
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BF358E-8660-487D-B01D-A7DC42B1C713}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A53C28B-DFA0-4A8C-8D93-CB40F81D2CEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1548,7 +1548,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1926,8 +1926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="C94" activeCellId="1" sqref="C89 C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3089,7 +3089,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="21">
-      <c r="A88">
+      <c r="A88" s="17">
         <v>79</v>
       </c>
       <c r="B88" s="3" t="s">

</xml_diff>

<commit_message>
80) Reorganize String added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C61234-F4E7-4650-8B96-4CDDE1B476CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BA6083-23EE-4C8C-B396-D7691C181A33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1926,8 +1926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3103,7 +3103,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" ht="21">
-      <c r="A89">
+      <c r="A89" s="16">
         <v>80</v>
       </c>
       <c r="B89" s="3" t="s">
@@ -3112,8 +3112,8 @@
       <c r="C89" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D89" s="10" t="s">
-        <v>4</v>
+      <c r="D89" s="11" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="21">
@@ -8438,375 +8438,375 @@
     <hyperlink ref="C85" r:id="rId75" xr:uid="{4A0E959E-22F4-6948-A819-76FE76AB9F6D}"/>
     <hyperlink ref="C86" r:id="rId76" xr:uid="{78B76678-D8EE-9745-98B1-DF7A76EA3B10}"/>
     <hyperlink ref="C87" r:id="rId77" xr:uid="{62982242-1D19-1544-8653-8E25E9BF4505}"/>
-    <hyperlink ref="C88" r:id="rId78" display="Write a program tofind the smallest window that contains all characters of string itself." xr:uid="{8E3D4BDF-9F8F-0542-BFD8-C3CE3BF396E6}"/>
-    <hyperlink ref="C89" r:id="rId79" xr:uid="{A3D51762-65A1-9A44-B619-D1D98A7F403B}"/>
-    <hyperlink ref="C90" r:id="rId80" xr:uid="{ED0F5FC7-0066-EB44-8FCF-460600DADB02}"/>
-    <hyperlink ref="C91" r:id="rId81" xr:uid="{2D956AC4-4774-7446-8473-C4CE00E33C17}"/>
-    <hyperlink ref="C92" r:id="rId82" xr:uid="{C8C607BB-1FEE-FA47-9E3E-6C0BCE978B7F}"/>
-    <hyperlink ref="C93" r:id="rId83" xr:uid="{B9AC5194-6D36-684A-A5C4-BEE11037599F}"/>
-    <hyperlink ref="C94" r:id="rId84" xr:uid="{AB28D9E6-890C-F14A-A5FB-2303BE319968}"/>
-    <hyperlink ref="C95" r:id="rId85" xr:uid="{1F507CBC-4056-AD46-9314-95ECBB9D799D}"/>
-    <hyperlink ref="C96" r:id="rId86" xr:uid="{F152A9AF-5CBA-EC44-A9CF-07AB481435AB}"/>
-    <hyperlink ref="C97" r:id="rId87" xr:uid="{346CA74F-60B7-0A4B-A612-9184D4DCFF62}"/>
-    <hyperlink ref="C98" r:id="rId88" xr:uid="{8C653CB1-4954-754F-8D46-F09141A2FCDB}"/>
-    <hyperlink ref="C101" r:id="rId89" xr:uid="{5989F693-2A61-A346-8395-8674307A4CC2}"/>
-    <hyperlink ref="C102" r:id="rId90" xr:uid="{3AD10C9E-4F6D-DE48-92F3-531A586520C6}"/>
-    <hyperlink ref="C103" r:id="rId91" xr:uid="{4FA217C0-A1F3-904E-8FEA-EA4941273A67}"/>
-    <hyperlink ref="C104" r:id="rId92" xr:uid="{A297BBC0-FA0D-2D46-9C49-3932193EF1D3}"/>
-    <hyperlink ref="C106" r:id="rId93" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance." xr:uid="{DCD751DE-E440-F346-B6FD-CBD072217214}"/>
-    <hyperlink ref="C107" r:id="rId94" xr:uid="{B2FD38B9-1E2B-8140-8291-F45734C98145}"/>
-    <hyperlink ref="C108" r:id="rId95" xr:uid="{C76888B3-18AC-9B48-9E2A-64A7DF0902B7}"/>
-    <hyperlink ref="C109" r:id="rId96" xr:uid="{18A79860-6C9E-A941-8D6C-360B9913E941}"/>
-    <hyperlink ref="C110" r:id="rId97" xr:uid="{C0DDFD68-CBC1-0F4A-AF40-ACF36BBC8453}"/>
-    <hyperlink ref="C111" r:id="rId98" xr:uid="{3E0BF737-E42E-C946-B32C-06882E0BA6FF}"/>
-    <hyperlink ref="C113" r:id="rId99" xr:uid="{862F9782-C57B-2848-A2D9-EB7B52FB7EC7}"/>
-    <hyperlink ref="C114" r:id="rId100" xr:uid="{230D7A6A-D2C5-C140-9A65-B1F407D22062}"/>
-    <hyperlink ref="C115" r:id="rId101" xr:uid="{BDC2BA28-4562-984E-8282-1126BF952EAF}"/>
-    <hyperlink ref="C116" r:id="rId102" xr:uid="{B53A5F28-6DED-3D47-8679-F78D3DDEFF01}"/>
-    <hyperlink ref="C117" r:id="rId103" xr:uid="{C57D0CC7-DA2F-0948-9BCE-F19C20C7D981}"/>
-    <hyperlink ref="C118" r:id="rId104" xr:uid="{117878E5-B8C8-254B-8ED6-014B4B7A8126}"/>
-    <hyperlink ref="C119" r:id="rId105" xr:uid="{B7CC0756-74F2-D54D-BDEE-9DA394DD7168}"/>
-    <hyperlink ref="C120" r:id="rId106" xr:uid="{837EF472-CCC2-CF47-A8A8-238E56F722CE}"/>
-    <hyperlink ref="C121" r:id="rId107" xr:uid="{3608F267-6AA0-624B-B243-7DDD317E9F08}"/>
-    <hyperlink ref="C122" r:id="rId108" xr:uid="{0B6123E6-0472-374B-ACA7-6914CD7918E8}"/>
-    <hyperlink ref="C123" r:id="rId109" xr:uid="{D3971CEB-C53E-B04B-9C32-1803182B5DC5}"/>
-    <hyperlink ref="C124" r:id="rId110" xr:uid="{7CF5013A-643E-1643-93A1-A2F1500D2A23}"/>
-    <hyperlink ref="C125" r:id="rId111" xr:uid="{2A6BE7E5-D818-6843-8C3E-99EA2BFE0FB2}"/>
-    <hyperlink ref="C126" r:id="rId112" xr:uid="{E718F544-96DF-A04E-8DFB-7639DA3EA57C}"/>
-    <hyperlink ref="C127" r:id="rId113" xr:uid="{B0C2F065-424A-7345-A864-346ECD98D749}"/>
-    <hyperlink ref="C128" r:id="rId114" xr:uid="{B4E26955-5C3F-804E-B19A-11260310AFB3}"/>
-    <hyperlink ref="C129" r:id="rId115" xr:uid="{6F299BB5-8E82-0240-A9A3-6829CE3ABCBF}"/>
-    <hyperlink ref="C130" r:id="rId116" xr:uid="{A42CA32F-2196-1840-A53D-E5073237C68D}"/>
-    <hyperlink ref="C131" r:id="rId117" xr:uid="{7ECF6EF4-962E-4642-9B1C-C3B70674793E}"/>
-    <hyperlink ref="C132" r:id="rId118" xr:uid="{2A109178-6B60-164E-9D25-42B3282137E3}"/>
-    <hyperlink ref="C133" r:id="rId119" xr:uid="{B3D38BD0-A6A1-8D41-8405-45E1BEEEEF06}"/>
-    <hyperlink ref="C134" r:id="rId120" xr:uid="{A1C26612-D040-2A41-A6A6-A8F2490C0A43}"/>
-    <hyperlink ref="C135" r:id="rId121" xr:uid="{C476E807-64CB-F44A-A23D-D21EBF6D001D}"/>
-    <hyperlink ref="C136" r:id="rId122" xr:uid="{9A414D55-D4A1-F147-9207-61B597D57136}"/>
-    <hyperlink ref="C105" r:id="rId123" xr:uid="{18B028A7-9B6F-D841-8548-924D70530779}"/>
-    <hyperlink ref="C112" r:id="rId124" xr:uid="{6D3E75EF-733F-7A4B-81C8-AEF6CB6335F0}"/>
-    <hyperlink ref="C139" r:id="rId125" xr:uid="{C9EB2682-BE0B-934B-B0B4-1DD1A1502647}"/>
-    <hyperlink ref="C140" r:id="rId126" xr:uid="{2992FED9-2B78-A342-92AA-E7C0F882FF17}"/>
-    <hyperlink ref="C141" r:id="rId127" xr:uid="{0084DA6F-EC84-BD48-BDA8-EBACA3BB3B3E}"/>
-    <hyperlink ref="C142" r:id="rId128" xr:uid="{30F2D415-4B2C-384C-8EAE-2CC71CB518E2}"/>
-    <hyperlink ref="C143" r:id="rId129" xr:uid="{40734C88-7C5B-9747-86D1-03463D9AD41A}"/>
-    <hyperlink ref="C144" r:id="rId130" xr:uid="{1040D22F-6729-104A-A229-CBDCED93024A}"/>
-    <hyperlink ref="C145" r:id="rId131" xr:uid="{E131FE61-FABF-8E4B-8EF0-F68379D8F836}"/>
-    <hyperlink ref="C146" r:id="rId132" xr:uid="{B2129272-1351-3745-883B-E6A7115450C8}"/>
-    <hyperlink ref="C147" r:id="rId133" xr:uid="{C8B2DEF0-2B69-C84E-8013-0B6F03FFC250}"/>
-    <hyperlink ref="C148" r:id="rId134" xr:uid="{536AC5CF-712F-BF48-94A9-D0E7DC013020}"/>
-    <hyperlink ref="C149" r:id="rId135" xr:uid="{2DABC9C7-43D4-1249-AF9B-5FA4552611CB}"/>
-    <hyperlink ref="C150" r:id="rId136" xr:uid="{DA62E73A-B495-F94A-BECE-D42E4CBF074A}"/>
-    <hyperlink ref="C151" r:id="rId137" xr:uid="{7F5E6966-850D-4F49-B2A5-678365713F28}"/>
-    <hyperlink ref="C152" r:id="rId138" xr:uid="{E9C4286D-8493-9A47-8B8C-09583FA72B70}"/>
-    <hyperlink ref="C153" r:id="rId139" xr:uid="{9EB0123C-84AE-1C4D-BA1A-C28CFB8EFB89}"/>
-    <hyperlink ref="C154" r:id="rId140" xr:uid="{9D11FED4-328F-674E-889D-EC781DD1D791}"/>
-    <hyperlink ref="C155" r:id="rId141" xr:uid="{48AE72DB-397B-464D-88AD-B8058ED29CC1}"/>
-    <hyperlink ref="C156" r:id="rId142" xr:uid="{152D50E9-7448-F542-AC66-05D0AE66664C}"/>
-    <hyperlink ref="C157" r:id="rId143" xr:uid="{34E6AF1B-5FB1-3A4B-8938-1DCF80831DC2}"/>
-    <hyperlink ref="C158" r:id="rId144" xr:uid="{E7F8B7CA-49F4-1946-91EE-E7582BE4E5DA}"/>
-    <hyperlink ref="C159" r:id="rId145" xr:uid="{3590A994-B7A2-C14D-9BF8-7AC8FE9E7F0F}"/>
-    <hyperlink ref="C160" r:id="rId146" xr:uid="{0AAA4B0C-4921-C34D-B41E-D702FA860892}"/>
-    <hyperlink ref="C161" r:id="rId147" xr:uid="{5973FCA4-AE32-5248-A6ED-2694367332F1}"/>
-    <hyperlink ref="C162" r:id="rId148" xr:uid="{4C0F816E-F043-0C47-BF16-1CDAD88D2FF1}"/>
-    <hyperlink ref="C163" r:id="rId149" xr:uid="{A8E4C654-D0BD-8945-9F5C-B09F7BC114BE}"/>
-    <hyperlink ref="C166" r:id="rId150" xr:uid="{E3825C15-10BB-E24F-B229-983F651DA942}"/>
-    <hyperlink ref="C167" r:id="rId151" xr:uid="{46ECFC31-388C-6241-8FFE-DED6F2FC794A}"/>
-    <hyperlink ref="C168" r:id="rId152" xr:uid="{589E024D-3FE1-1048-890C-88289733F233}"/>
-    <hyperlink ref="C169" r:id="rId153" xr:uid="{CDA28F7A-7FC5-F74D-B27E-A6E0161D41D5}"/>
-    <hyperlink ref="C170" r:id="rId154" xr:uid="{DA6A0D92-DCEB-DA4F-8BBA-10FCD092838F}"/>
-    <hyperlink ref="C171" r:id="rId155" xr:uid="{955769DB-3256-254B-90DE-E1E01B272F8A}"/>
-    <hyperlink ref="C172" r:id="rId156" xr:uid="{DED7AC9B-40D7-0545-9D6F-6CD4F5FFE4C6}"/>
-    <hyperlink ref="C173" r:id="rId157" xr:uid="{6947A4E1-B6AA-6D4F-A6D8-8FA74FD02887}"/>
-    <hyperlink ref="C174" r:id="rId158" xr:uid="{EABF2012-5A90-0C4E-86F6-FDB5FA7770BE}"/>
-    <hyperlink ref="C177" r:id="rId159" xr:uid="{7F44CFE0-9ED1-A44D-B9EF-CF87BEB644FC}"/>
-    <hyperlink ref="C178" r:id="rId160" xr:uid="{CF6E0CF6-7A93-D84A-9CE0-5BDD51767416}"/>
-    <hyperlink ref="C179" r:id="rId161" xr:uid="{EFF8F154-60B8-B84B-84CA-32756BD6430F}"/>
-    <hyperlink ref="C180" r:id="rId162" xr:uid="{C8A3094E-E11B-2543-B05E-1D07048B2EBA}"/>
-    <hyperlink ref="C181" r:id="rId163" xr:uid="{9961E5F5-B5C6-0C4D-A1D0-D04D2A5D7DFD}"/>
-    <hyperlink ref="C182" r:id="rId164" xr:uid="{44E289EC-47DD-D94D-88C1-CB2F59C6C16A}"/>
-    <hyperlink ref="C183" r:id="rId165" xr:uid="{4161FC70-DD6D-684B-898A-A4711596B2D5}"/>
-    <hyperlink ref="C184" r:id="rId166" xr:uid="{B9CBE387-8E9A-ED48-8310-CF7D34FA690C}"/>
-    <hyperlink ref="C185" r:id="rId167" xr:uid="{5398097B-24FF-9543-8F02-33CE2860F1F7}"/>
-    <hyperlink ref="C186" r:id="rId168" xr:uid="{3B1FC30B-30C8-7B48-AF94-A81FB513F24F}"/>
-    <hyperlink ref="C187" r:id="rId169" xr:uid="{32B750D0-D7F2-694D-AB9B-25AFAFAFF17F}"/>
-    <hyperlink ref="C188" r:id="rId170" xr:uid="{400689DD-8E95-024E-976B-AACD8ED4E1A6}"/>
-    <hyperlink ref="C189" r:id="rId171" xr:uid="{28753DDE-E047-5D40-A30B-1103BE6DA08F}"/>
-    <hyperlink ref="C190" r:id="rId172" xr:uid="{6C5AA6CB-3D93-0740-AEED-9E6C218CF6CB}"/>
-    <hyperlink ref="C191" r:id="rId173" xr:uid="{03EAA2B9-D8B8-D642-BF24-380596D26B2E}"/>
-    <hyperlink ref="C192" r:id="rId174" xr:uid="{8C1719B4-37CC-484E-BDCE-A4272C07F91B}"/>
-    <hyperlink ref="C193" r:id="rId175" xr:uid="{6C198DA2-BB98-F940-8EF6-2FC8B7AE577A}"/>
-    <hyperlink ref="C194" r:id="rId176" xr:uid="{AB0EA311-A446-D046-A0EC-290B42068328}"/>
-    <hyperlink ref="C195" r:id="rId177" xr:uid="{DB913045-B9F6-6549-AA09-22B0CC5FDD21}"/>
-    <hyperlink ref="C196" r:id="rId178" xr:uid="{806469FD-617A-7445-AAB5-FB2FD2ED24EA}"/>
-    <hyperlink ref="C197" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{1A10544E-58CF-D04D-9FAF-2FEC6DB2B5D4}"/>
-    <hyperlink ref="C198" r:id="rId180" xr:uid="{5A0B6645-89FD-E044-A706-9FB890274C3C}"/>
-    <hyperlink ref="C199" r:id="rId181" xr:uid="{B42A3009-E8EB-EE44-885F-6699C17A0E0B}"/>
-    <hyperlink ref="C200" r:id="rId182" xr:uid="{ED3E48AB-E25B-3744-B024-E97B2A319B46}"/>
-    <hyperlink ref="C201" r:id="rId183" xr:uid="{C75D20A3-CBAE-2649-A3EE-E49177CFA343}"/>
-    <hyperlink ref="C202" r:id="rId184" xr:uid="{3863CA1B-D43E-1144-91A9-17C2DCF52A64}"/>
-    <hyperlink ref="C203" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{E9AF434E-4CAA-5D49-8AD3-889CDE2913D9}"/>
-    <hyperlink ref="C204" r:id="rId186" xr:uid="{1A0568E5-3A11-7F47-8001-82B05D7C2339}"/>
-    <hyperlink ref="C205" r:id="rId187" xr:uid="{F62B8AE4-9C4F-9544-8861-CD733C12F79E}"/>
-    <hyperlink ref="C206" r:id="rId188" xr:uid="{0F6A542C-44C9-5A4C-90BF-BC8C239877D2}"/>
-    <hyperlink ref="C207" r:id="rId189" xr:uid="{3ED28203-B1B5-4E46-AAF3-779EDD4AC03F}"/>
-    <hyperlink ref="C208" r:id="rId190" xr:uid="{4338B305-B52F-5540-9B51-B938FC6803A2}"/>
-    <hyperlink ref="C209" r:id="rId191" xr:uid="{DDEEED0F-A939-1E4F-B2FA-AD391A4A2874}"/>
-    <hyperlink ref="C210" r:id="rId192" xr:uid="{C2F20589-AD81-654C-94E5-E5B6C9FE27F6}"/>
-    <hyperlink ref="C211" r:id="rId193" xr:uid="{BBEB9DAC-E4AE-C04F-AA15-6356AFC57FDE}"/>
-    <hyperlink ref="C214" r:id="rId194" xr:uid="{6316566D-A10A-F849-9F25-B9ED4DA12BC7}"/>
-    <hyperlink ref="C215" r:id="rId195" xr:uid="{9D4DD895-FBA6-C849-A5BF-3B30755BD9C9}"/>
-    <hyperlink ref="C216" r:id="rId196" xr:uid="{475996DA-632A-BE49-AEA1-D4189FD614A1}"/>
-    <hyperlink ref="C217" r:id="rId197" xr:uid="{88E0C858-8468-884F-BB71-F6F176BD5FC2}"/>
-    <hyperlink ref="C218" r:id="rId198" xr:uid="{C1C5C8D0-7A06-3D4A-A85A-AAACC1B418C9}"/>
-    <hyperlink ref="C219" r:id="rId199" xr:uid="{D525D4B1-2857-1543-8CD9-196728321203}"/>
-    <hyperlink ref="C220" r:id="rId200" xr:uid="{51E3AB9B-04B2-C041-A2B3-37E3EB18013A}"/>
-    <hyperlink ref="C221" r:id="rId201" xr:uid="{7F7F0C9A-57B9-314F-959A-B8ACAFA5FD13}"/>
-    <hyperlink ref="C222" r:id="rId202" xr:uid="{3B029785-83B4-6140-8B70-CD892CFC87F6}"/>
-    <hyperlink ref="C223" r:id="rId203" xr:uid="{B0A390E6-D860-9F4E-B021-68949FE712F3}"/>
-    <hyperlink ref="C224" r:id="rId204" xr:uid="{49E9953D-52F6-BF47-8AAA-8E456F55576B}"/>
-    <hyperlink ref="C225" r:id="rId205" xr:uid="{9B812470-F419-A54E-8365-06A9B8864A30}"/>
-    <hyperlink ref="C226" r:id="rId206" xr:uid="{B6FB4107-1933-6D45-9EF4-4474E06CBE9D}"/>
-    <hyperlink ref="C227" r:id="rId207" xr:uid="{0F7C1D92-7BCB-D14D-A658-9599984E04E4}"/>
-    <hyperlink ref="C228" r:id="rId208" xr:uid="{6810428F-0A78-964C-A8C8-E1CD2E7C405D}"/>
-    <hyperlink ref="C229" r:id="rId209" xr:uid="{B40209F2-0D6E-364F-8AF6-F1D182509314}"/>
-    <hyperlink ref="C230" r:id="rId210" xr:uid="{96C53FA9-9FD3-2D4F-B292-3C9DEDFA806E}"/>
-    <hyperlink ref="C231" r:id="rId211" xr:uid="{918B420D-3678-FD46-9463-595E8ACC39E1}"/>
-    <hyperlink ref="C232" r:id="rId212" xr:uid="{851A7153-3B54-0E4A-A0A0-FCEB091AFE70}"/>
-    <hyperlink ref="C233" r:id="rId213" xr:uid="{C03AE9F8-09AE-C640-81A7-033BB06FB6AD}"/>
-    <hyperlink ref="C234" r:id="rId214" xr:uid="{35140DEB-52D2-4342-88D2-22BA061E5B48}"/>
-    <hyperlink ref="C235" r:id="rId215" xr:uid="{9714BC0B-3373-934C-B7A1-599F74F4FB9D}"/>
-    <hyperlink ref="C238" r:id="rId216" xr:uid="{5CB435B2-7FD2-1D44-9872-22B6A1EDC02B}"/>
-    <hyperlink ref="C239" r:id="rId217" xr:uid="{722D1D95-896B-4642-BABD-31DEDD237B49}"/>
-    <hyperlink ref="C240" r:id="rId218" xr:uid="{D686D1DC-13D6-284C-B606-E087FAF47399}"/>
-    <hyperlink ref="C241" r:id="rId219" xr:uid="{D22C2394-C3CB-8F4F-A010-2B13C8C84D1A}"/>
-    <hyperlink ref="C242" r:id="rId220" xr:uid="{3AE2F800-B66F-1A41-893B-978F6875FDC8}"/>
-    <hyperlink ref="C243" r:id="rId221" xr:uid="{2C939BDE-5298-5541-837B-8C59D53A33C1}"/>
-    <hyperlink ref="C244" r:id="rId222" xr:uid="{691C9BD8-69D3-DA4B-AEB6-AF827B4ACA9F}"/>
-    <hyperlink ref="C245" r:id="rId223" xr:uid="{B6891E82-7C4D-424D-9219-3C9FD08E0053}"/>
-    <hyperlink ref="C246" r:id="rId224" xr:uid="{67A1AE98-62D2-644D-AC13-6CD76CF53CC0}"/>
-    <hyperlink ref="C247" r:id="rId225" xr:uid="{B59D4881-2A82-8F4D-B151-1E796C4923C8}"/>
-    <hyperlink ref="C248" r:id="rId226" xr:uid="{B3CBD023-5EFD-6048-9B3F-89F0C65CBBF5}"/>
-    <hyperlink ref="C249" r:id="rId227" xr:uid="{53EC42C4-22F7-0445-A0AC-7275A59A2672}"/>
-    <hyperlink ref="C250" r:id="rId228" xr:uid="{A29575F3-CB24-5B4B-9538-D5212B2DC28B}"/>
-    <hyperlink ref="C251" r:id="rId229" xr:uid="{353A44DD-9E30-8F48-8E2B-8DAA07550470}"/>
-    <hyperlink ref="C252" r:id="rId230" xr:uid="{32AC291D-95A5-BE49-88E0-02677BF39CAC}"/>
-    <hyperlink ref="C253" r:id="rId231" xr:uid="{A84F22FF-AD10-A546-8998-B066C0EB2D5A}"/>
-    <hyperlink ref="C254" r:id="rId232" xr:uid="{4C5CAF84-9B94-FC44-8C6C-B3CC7257C1DB}"/>
-    <hyperlink ref="C255" r:id="rId233" xr:uid="{5DA775E2-C516-3B47-8C82-3CEE7CC0BDF9}"/>
-    <hyperlink ref="C256" r:id="rId234" xr:uid="{00B6AE5C-EF3F-0747-A280-3BF055362B4F}"/>
-    <hyperlink ref="C257" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{BCBD0A7E-F3D0-E840-9375-AFD37C5CD41A}"/>
-    <hyperlink ref="C258" r:id="rId236" xr:uid="{47ABDDDB-F95F-8049-9FB3-1E71A7376DDE}"/>
-    <hyperlink ref="C259" r:id="rId237" xr:uid="{70BADFC9-7399-234D-99F6-4C5F02397C26}"/>
-    <hyperlink ref="C260" r:id="rId238" xr:uid="{63348580-70EF-EC47-BF49-8ECE9560D54E}"/>
-    <hyperlink ref="C261" r:id="rId239" xr:uid="{D5BD96B3-9EAB-1B47-AC87-5C47F6AD7F40}"/>
-    <hyperlink ref="C262" r:id="rId240" xr:uid="{74791141-3FB8-7540-B45B-9541AF0AE371}"/>
-    <hyperlink ref="C263" r:id="rId241" xr:uid="{88D53CD6-262A-7247-8E58-FE9FFF7ECC40}"/>
-    <hyperlink ref="C264" r:id="rId242" xr:uid="{4338A14D-4F7D-B943-A347-7F74EFCA0DB5}"/>
-    <hyperlink ref="C265" r:id="rId243" xr:uid="{6E0EF7A3-7341-284B-A0E3-4539B6EAFAF2}"/>
-    <hyperlink ref="C266" r:id="rId244" xr:uid="{D2D8D64F-E2D3-734E-AD45-3EFB9686555A}"/>
-    <hyperlink ref="C267" r:id="rId245" xr:uid="{04A2904A-73A0-7845-9868-2CCFE359AC68}"/>
-    <hyperlink ref="C268" r:id="rId246" xr:uid="{D3D35835-6BE3-4D41-AF6F-5FE442277A16}"/>
-    <hyperlink ref="C269" r:id="rId247" xr:uid="{F663D0FC-CFF0-BC4F-9D26-48C871A8E9FD}"/>
-    <hyperlink ref="C270" r:id="rId248" xr:uid="{DF544147-DA48-4041-A4E2-4A75106B771A}"/>
-    <hyperlink ref="C271" r:id="rId249" xr:uid="{50E4B716-239E-7946-843D-E8462591D128}"/>
-    <hyperlink ref="C272" r:id="rId250" xr:uid="{D368B3E5-7D12-FD48-AFF7-A4A614108940}"/>
-    <hyperlink ref="C275" r:id="rId251" xr:uid="{D5921FF1-FC1F-CA4B-A24E-AD69E1DEC14C}"/>
-    <hyperlink ref="C276" r:id="rId252" xr:uid="{C931D7E0-E032-7C4B-95F1-735D955FCB51}"/>
-    <hyperlink ref="C277" r:id="rId253" xr:uid="{5FBD4A8F-287C-2C46-9CAB-F7DBA67DEDDA}"/>
-    <hyperlink ref="C278" r:id="rId254" xr:uid="{12966DD6-41DD-A94B-8B2C-0AD7D2AD6FB0}"/>
-    <hyperlink ref="C279" r:id="rId255" xr:uid="{CF720C34-4554-2944-A818-020ABC9BF0F4}"/>
-    <hyperlink ref="C280" r:id="rId256" xr:uid="{75763F2A-16D7-DE43-8189-19623CE26370}"/>
-    <hyperlink ref="C281" r:id="rId257" xr:uid="{9263AA30-472A-0A4D-BADF-96D82BB9BFCC}"/>
-    <hyperlink ref="C282" r:id="rId258" xr:uid="{2EF025C3-75C8-564E-BA8B-708C32B0E602}"/>
-    <hyperlink ref="C283" r:id="rId259" xr:uid="{6BDFDCA9-3421-F24F-8EF2-A72742F0AC21}"/>
-    <hyperlink ref="C284" r:id="rId260" xr:uid="{D8447F99-5FF9-D544-99BB-E9969B4A38D7}"/>
-    <hyperlink ref="C285" r:id="rId261" xr:uid="{1DB7EFDA-6C7D-F546-9EE1-F61ED0F65209}"/>
-    <hyperlink ref="C286" r:id="rId262" xr:uid="{D1505609-27D1-784D-ACF6-AE9D0DA2E1B6}"/>
-    <hyperlink ref="C287" r:id="rId263" xr:uid="{6BFA7B45-17D0-4E49-85DA-23C7255A306D}"/>
-    <hyperlink ref="C288" r:id="rId264" xr:uid="{3324BA4A-30CA-5246-8C3C-6505A6987939}"/>
-    <hyperlink ref="C289" r:id="rId265" xr:uid="{894486AD-2B6D-5740-BCAF-0BA1AFF814B4}"/>
-    <hyperlink ref="C290" r:id="rId266" xr:uid="{C47B203B-8B5A-E740-8C86-0784AD28089E}"/>
-    <hyperlink ref="C291" r:id="rId267" xr:uid="{06DC2E54-7597-AE4D-ACDB-B8883A989A4F}"/>
-    <hyperlink ref="C292" r:id="rId268" xr:uid="{E3384259-7CA7-1C44-A66D-11346EE6742E}"/>
-    <hyperlink ref="C293" r:id="rId269" xr:uid="{A5B77769-38AF-3D47-A76B-311591B57D91}"/>
-    <hyperlink ref="C296" r:id="rId270" xr:uid="{9DB6976A-C646-1341-90E8-3A164521267A}"/>
-    <hyperlink ref="C297" r:id="rId271" xr:uid="{03C291F8-D19A-304B-9EF9-CF71A1F66E49}"/>
-    <hyperlink ref="C298" r:id="rId272" xr:uid="{7536415C-140B-9244-B0B2-23F3ED0B2D80}"/>
-    <hyperlink ref="C299" r:id="rId273" xr:uid="{7DBDA456-8AF6-DD43-9764-17D3959B8E8F}"/>
-    <hyperlink ref="C300" r:id="rId274" xr:uid="{BFC149AB-C15A-B648-9F6A-ECD3890B1918}"/>
-    <hyperlink ref="C301" r:id="rId275" xr:uid="{0482240B-FEE9-F746-8980-52BCB7BBB56E}"/>
-    <hyperlink ref="C302" r:id="rId276" xr:uid="{86D1231A-E7C8-4B45-99ED-2DB0EF71E190}"/>
-    <hyperlink ref="C303" r:id="rId277" xr:uid="{20B7CE89-CB37-0040-989F-C8D1BE2B8782}"/>
-    <hyperlink ref="C304" r:id="rId278" xr:uid="{4C8412C9-A47B-9244-A18B-741516BD1054}"/>
-    <hyperlink ref="C305" r:id="rId279" xr:uid="{511761D9-31CE-0B43-AFFD-C011C27ACC52}"/>
-    <hyperlink ref="C306" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{6905F997-D048-1049-BA27-C48756603D1E}"/>
-    <hyperlink ref="C307" r:id="rId281" xr:uid="{E657AA82-7CFE-DB42-B20F-F63D8C25EAB6}"/>
-    <hyperlink ref="C308" r:id="rId282" xr:uid="{3E505033-58F3-8F4E-AB82-E12DBC226AEA}"/>
-    <hyperlink ref="C309" r:id="rId283" xr:uid="{749599E5-4972-7343-B13B-87E26F837470}"/>
-    <hyperlink ref="C310" r:id="rId284" xr:uid="{12AA88DC-22AB-5A49-B28C-F04C8E35A215}"/>
-    <hyperlink ref="C311" r:id="rId285" xr:uid="{5751F0A7-7D9D-4148-820B-5B9659DFE34F}"/>
-    <hyperlink ref="C312" r:id="rId286" xr:uid="{4CA2DBEE-B161-B84D-B3A9-B8BC1B598AF2}"/>
-    <hyperlink ref="C313" r:id="rId287" xr:uid="{A9C1E578-6594-954C-8785-8902E605FC7A}"/>
-    <hyperlink ref="C314" r:id="rId288" xr:uid="{3D45E9B8-6671-A747-8C18-51CF8883170A}"/>
-    <hyperlink ref="C315" r:id="rId289" xr:uid="{4F5EF748-8CD4-0F47-90CE-3C93755BF63D}"/>
-    <hyperlink ref="C316" r:id="rId290" xr:uid="{44053C08-5050-C84B-B016-069B1EF9A43D}"/>
-    <hyperlink ref="C317" r:id="rId291" xr:uid="{ABF38928-736B-1A49-8B8A-1DCA5AAECB2B}"/>
-    <hyperlink ref="C318" r:id="rId292" xr:uid="{52651FAF-F3DC-E949-8AF8-998B9724B7D1}"/>
-    <hyperlink ref="C319" r:id="rId293" xr:uid="{91C6CCEF-3FF7-2C42-B5A0-8F4A403ED198}"/>
-    <hyperlink ref="C320" r:id="rId294" xr:uid="{15C8AF08-1A79-F949-9BE7-DD240CBD9861}"/>
-    <hyperlink ref="C321" r:id="rId295" xr:uid="{1904F984-5B22-8D46-BC33-3073B390E8F9}"/>
-    <hyperlink ref="C322" r:id="rId296" xr:uid="{A8BFB3A4-426B-E646-BCF0-FE19C8CD07A9}"/>
-    <hyperlink ref="C323" r:id="rId297" xr:uid="{FBBA29BB-885B-744A-A644-58EDCA7B140A}"/>
-    <hyperlink ref="C324" r:id="rId298" xr:uid="{75411687-6884-AC42-8B4A-1348C4837365}"/>
-    <hyperlink ref="C325" r:id="rId299" xr:uid="{A89ED8DF-F678-FE43-808C-C190721379BF}"/>
-    <hyperlink ref="C326" r:id="rId300" xr:uid="{1516834D-F3B2-1743-8811-263E11BBDEF8}"/>
-    <hyperlink ref="C327" r:id="rId301" xr:uid="{1659AB91-08CA-E44D-988D-E9D9A746D406}"/>
-    <hyperlink ref="C328" r:id="rId302" xr:uid="{E844BC1D-9713-9F4D-B0A4-1124A9952D14}"/>
-    <hyperlink ref="C329" r:id="rId303" xr:uid="{DCE2AAEF-8D8E-1843-BFE9-E9B7E13854EB}"/>
-    <hyperlink ref="C330" r:id="rId304" xr:uid="{836B3BF0-7711-7D41-9E72-914C1871397F}"/>
-    <hyperlink ref="C331" r:id="rId305" xr:uid="{F450CF9B-CA59-1443-8163-13F1121DCF12}"/>
-    <hyperlink ref="C332" r:id="rId306" xr:uid="{1539C3E8-4854-3C4F-A7B3-55BF931F1E2A}"/>
-    <hyperlink ref="C333" r:id="rId307" xr:uid="{04F1FC5F-5DA1-0144-962D-B38C1C41F0F4}"/>
-    <hyperlink ref="C336" r:id="rId308" xr:uid="{B21618F4-70E2-C549-80B7-7CF915679E0A}"/>
-    <hyperlink ref="C337" r:id="rId309" xr:uid="{EEDFBF11-C1E4-0847-9D56-94A72D97AEE7}"/>
-    <hyperlink ref="C338" r:id="rId310" xr:uid="{F5C0EDF1-7EAC-8849-8D27-C3389913BFC6}"/>
-    <hyperlink ref="C339" r:id="rId311" xr:uid="{50175B29-124F-4E4E-8E98-961BD3320359}"/>
-    <hyperlink ref="C340" r:id="rId312" xr:uid="{1BE23822-8512-014F-9154-F6EDA4FC8428}"/>
-    <hyperlink ref="C341" r:id="rId313" xr:uid="{38EC228E-ABFF-3542-9CFB-3DDFC628E9D0}"/>
-    <hyperlink ref="C342" r:id="rId314" xr:uid="{73F240F8-C469-454E-BA5C-CFF2F7A7A5F6}"/>
-    <hyperlink ref="C343" r:id="rId315" xr:uid="{3BBD1BAC-68C7-A94A-9063-AF62B5C837FD}"/>
-    <hyperlink ref="C344" r:id="rId316" xr:uid="{F9751D9B-2689-E24B-9FC3-CA32FE888708}"/>
-    <hyperlink ref="C345" r:id="rId317" xr:uid="{73C61D6A-D97C-B944-8B27-BB91564AB0D7}"/>
-    <hyperlink ref="C346" r:id="rId318" xr:uid="{936E077C-C016-A04F-895A-782D6D9D9433}"/>
-    <hyperlink ref="C347" r:id="rId319" xr:uid="{5454A2A1-6607-BE48-9215-CB8965EC3568}"/>
-    <hyperlink ref="C348" r:id="rId320" xr:uid="{FC1EAA10-F7ED-6B42-A79B-3D8B44E2C8B3}"/>
-    <hyperlink ref="C349" r:id="rId321" xr:uid="{FDB7F712-4A42-1048-8929-A1E752B07C6A}"/>
-    <hyperlink ref="C350" r:id="rId322" xr:uid="{AF3ACA60-0B0E-E146-B51F-A2CD05EB6549}"/>
-    <hyperlink ref="C351" r:id="rId323" xr:uid="{BB63E040-7A1A-E046-9BDD-9CBD1DA89DE9}"/>
-    <hyperlink ref="C352" r:id="rId324" xr:uid="{9AF8FD93-CCC9-D540-AE9A-00583F309649}"/>
-    <hyperlink ref="C353" r:id="rId325" xr:uid="{66A746A0-71FE-E546-92B7-D1C3D582E067}"/>
-    <hyperlink ref="C357" r:id="rId326" xr:uid="{BD79CCE1-5315-3944-9F9B-618615EC4583}"/>
-    <hyperlink ref="C358" r:id="rId327" xr:uid="{A5068A51-C961-6847-BB27-40A850B6D393}"/>
-    <hyperlink ref="C359" r:id="rId328" xr:uid="{6B8D36F0-E796-B944-A456-E8A9E2EE0BDB}"/>
-    <hyperlink ref="C360" r:id="rId329" xr:uid="{776652B7-2C11-4641-BF6A-EABEEB9B55AB}"/>
-    <hyperlink ref="C361" r:id="rId330" xr:uid="{95C6B35D-712A-2343-B790-236B55C5EC49}"/>
-    <hyperlink ref="C362" r:id="rId331" xr:uid="{4ED53872-1FE9-F140-AA35-F228F762880B}"/>
-    <hyperlink ref="C363" r:id="rId332" xr:uid="{6D5E6A28-85AA-BF4C-B2BD-9378D6E28EC7}"/>
-    <hyperlink ref="C364" r:id="rId333" xr:uid="{BCAD1ECB-15EE-CF49-878E-AA682DE3AC22}"/>
-    <hyperlink ref="C365" r:id="rId334" xr:uid="{C85468B5-25E9-E446-808E-72CFE911F0C2}"/>
-    <hyperlink ref="C366" r:id="rId335" xr:uid="{9503AECA-1A6A-9640-A04C-4CEAA2304448}"/>
-    <hyperlink ref="C367" r:id="rId336" xr:uid="{74211516-06B0-AA45-845B-52C8202751DA}"/>
-    <hyperlink ref="C368" r:id="rId337" xr:uid="{02C696BC-4B91-9444-900F-9CD68E409ABC}"/>
-    <hyperlink ref="C369" r:id="rId338" xr:uid="{04646C45-4118-374C-839D-94D31D534FAC}"/>
-    <hyperlink ref="C370" r:id="rId339" xr:uid="{F90BCCAE-8596-FC4D-BDD7-774392C596DF}"/>
-    <hyperlink ref="C371" r:id="rId340" xr:uid="{65230925-36EC-8A4B-8E46-6350B9BC0F95}"/>
-    <hyperlink ref="C372" r:id="rId341" xr:uid="{E91B8177-0C7A-1F40-BD34-4CC60F03B84F}"/>
-    <hyperlink ref="C373" r:id="rId342" xr:uid="{E8CBFD60-7335-0B4D-9FF5-99B4A8DC551D}"/>
-    <hyperlink ref="C374" r:id="rId343" xr:uid="{A35F55D4-9B87-C745-94DB-E7D820193C30}"/>
-    <hyperlink ref="C375" r:id="rId344" xr:uid="{6461A29F-D404-334F-B13F-296B4CA5E8A4}"/>
-    <hyperlink ref="C376" r:id="rId345" xr:uid="{FA9B4BE7-85CC-B24F-9461-5E9B42DDD824}"/>
-    <hyperlink ref="C377" r:id="rId346" xr:uid="{A75ACEA2-CDF6-A147-8540-A6DF55B15F45}"/>
-    <hyperlink ref="C378" r:id="rId347" xr:uid="{62FF87E2-E658-AB4D-AC57-7BCF9D49516E}"/>
-    <hyperlink ref="C379" r:id="rId348" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{269338A6-5145-6944-9F7F-BD2A86DFA308}"/>
-    <hyperlink ref="C380" r:id="rId349" xr:uid="{8F583049-CE8D-CD42-88CD-CF3857942670}"/>
-    <hyperlink ref="C381" r:id="rId350" xr:uid="{EE2348AD-E296-894A-B5AE-5884A3C5E419}"/>
-    <hyperlink ref="C382" r:id="rId351" xr:uid="{6EACB34E-B32E-8F43-8055-2406F7417A7E}"/>
-    <hyperlink ref="C383" r:id="rId352" xr:uid="{2446F10A-B762-B64C-97B2-6131A0BECC1F}"/>
-    <hyperlink ref="C384" r:id="rId353" xr:uid="{6FDFCC53-17A6-7244-88A7-49406D7C9200}"/>
-    <hyperlink ref="C385" r:id="rId354" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
-    <hyperlink ref="C386" r:id="rId355" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
-    <hyperlink ref="C387" r:id="rId356" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
-    <hyperlink ref="C388" r:id="rId357" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
-    <hyperlink ref="C389" r:id="rId358" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
-    <hyperlink ref="C390" r:id="rId359" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
-    <hyperlink ref="C391" r:id="rId360" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
-    <hyperlink ref="C392" r:id="rId361" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
-    <hyperlink ref="C393" r:id="rId362" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
-    <hyperlink ref="C394" r:id="rId363" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
-    <hyperlink ref="C396" r:id="rId364" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
-    <hyperlink ref="C395" r:id="rId365" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
-    <hyperlink ref="C397" r:id="rId366" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
-    <hyperlink ref="C398" r:id="rId367" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
-    <hyperlink ref="C399" r:id="rId368" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
-    <hyperlink ref="C402" r:id="rId369" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
-    <hyperlink ref="C403" r:id="rId370" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
-    <hyperlink ref="C404" r:id="rId371" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
-    <hyperlink ref="C405" r:id="rId372" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
-    <hyperlink ref="C406" r:id="rId373" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
-    <hyperlink ref="C407" r:id="rId374" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
-    <hyperlink ref="C410" r:id="rId375" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
-    <hyperlink ref="C411" r:id="rId376" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
-    <hyperlink ref="C412" r:id="rId377" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
-    <hyperlink ref="C413" r:id="rId378" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
-    <hyperlink ref="C414" r:id="rId379" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
-    <hyperlink ref="C415" r:id="rId380" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
-    <hyperlink ref="C416" r:id="rId381" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
-    <hyperlink ref="C417" r:id="rId382" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
-    <hyperlink ref="C418" r:id="rId383" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
-    <hyperlink ref="C419" r:id="rId384" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
-    <hyperlink ref="C420" r:id="rId385" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
-    <hyperlink ref="C421" r:id="rId386" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
-    <hyperlink ref="C422" r:id="rId387" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
-    <hyperlink ref="C423" r:id="rId388" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
-    <hyperlink ref="C424" r:id="rId389" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
-    <hyperlink ref="C425" r:id="rId390" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
-    <hyperlink ref="C426" r:id="rId391" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
-    <hyperlink ref="C427" r:id="rId392" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
-    <hyperlink ref="C428" r:id="rId393" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
-    <hyperlink ref="C429" r:id="rId394" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
-    <hyperlink ref="C430" r:id="rId395" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
-    <hyperlink ref="C431" r:id="rId396" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
-    <hyperlink ref="C432" r:id="rId397" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
-    <hyperlink ref="C433" r:id="rId398" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
-    <hyperlink ref="C434" r:id="rId399" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
-    <hyperlink ref="C435" r:id="rId400" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
-    <hyperlink ref="C436" r:id="rId401" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
-    <hyperlink ref="C437" r:id="rId402" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
-    <hyperlink ref="C438" r:id="rId403" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
-    <hyperlink ref="C439" r:id="rId404" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
-    <hyperlink ref="C440" r:id="rId405" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
-    <hyperlink ref="C441" r:id="rId406" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
-    <hyperlink ref="C442" r:id="rId407" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
-    <hyperlink ref="C443" r:id="rId408" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
-    <hyperlink ref="C444" r:id="rId409" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
-    <hyperlink ref="C445" r:id="rId410" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
-    <hyperlink ref="C446" r:id="rId411" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
-    <hyperlink ref="C447" r:id="rId412" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
-    <hyperlink ref="C448" r:id="rId413" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
-    <hyperlink ref="C449" r:id="rId414" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
-    <hyperlink ref="C451" r:id="rId415" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
-    <hyperlink ref="C450" r:id="rId416" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
-    <hyperlink ref="C452" r:id="rId417" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
-    <hyperlink ref="C453" r:id="rId418" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
-    <hyperlink ref="C454" r:id="rId419" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
-    <hyperlink ref="C455" r:id="rId420" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
-    <hyperlink ref="C456" r:id="rId421" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
-    <hyperlink ref="C457" r:id="rId422" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
-    <hyperlink ref="C458" r:id="rId423" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
-    <hyperlink ref="C459" r:id="rId424" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
-    <hyperlink ref="C460" r:id="rId425" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
-    <hyperlink ref="C461" r:id="rId426" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
-    <hyperlink ref="C462" r:id="rId427" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
-    <hyperlink ref="C469" r:id="rId428" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
-    <hyperlink ref="C468" r:id="rId429" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
-    <hyperlink ref="C467" r:id="rId430" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
-    <hyperlink ref="C466" r:id="rId431" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
-    <hyperlink ref="C465" r:id="rId432" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
-    <hyperlink ref="C464" r:id="rId433" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
-    <hyperlink ref="C463" r:id="rId434" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
-    <hyperlink ref="C472" r:id="rId435" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
-    <hyperlink ref="C473" r:id="rId436" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
-    <hyperlink ref="C474" r:id="rId437" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
-    <hyperlink ref="C475" r:id="rId438" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
-    <hyperlink ref="C476" r:id="rId439" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
-    <hyperlink ref="C477" r:id="rId440" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
-    <hyperlink ref="C478" r:id="rId441" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
-    <hyperlink ref="C481" r:id="rId442" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
-    <hyperlink ref="C479" r:id="rId443" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
-    <hyperlink ref="C480" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
-    <hyperlink ref="C356" r:id="rId445" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
-    <hyperlink ref="C2" r:id="rId446" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
+    <hyperlink ref="C89" r:id="rId78" xr:uid="{A3D51762-65A1-9A44-B619-D1D98A7F403B}"/>
+    <hyperlink ref="C90" r:id="rId79" xr:uid="{ED0F5FC7-0066-EB44-8FCF-460600DADB02}"/>
+    <hyperlink ref="C91" r:id="rId80" xr:uid="{2D956AC4-4774-7446-8473-C4CE00E33C17}"/>
+    <hyperlink ref="C92" r:id="rId81" xr:uid="{C8C607BB-1FEE-FA47-9E3E-6C0BCE978B7F}"/>
+    <hyperlink ref="C93" r:id="rId82" xr:uid="{B9AC5194-6D36-684A-A5C4-BEE11037599F}"/>
+    <hyperlink ref="C94" r:id="rId83" xr:uid="{AB28D9E6-890C-F14A-A5FB-2303BE319968}"/>
+    <hyperlink ref="C95" r:id="rId84" xr:uid="{1F507CBC-4056-AD46-9314-95ECBB9D799D}"/>
+    <hyperlink ref="C96" r:id="rId85" xr:uid="{F152A9AF-5CBA-EC44-A9CF-07AB481435AB}"/>
+    <hyperlink ref="C97" r:id="rId86" xr:uid="{346CA74F-60B7-0A4B-A612-9184D4DCFF62}"/>
+    <hyperlink ref="C98" r:id="rId87" xr:uid="{8C653CB1-4954-754F-8D46-F09141A2FCDB}"/>
+    <hyperlink ref="C101" r:id="rId88" xr:uid="{5989F693-2A61-A346-8395-8674307A4CC2}"/>
+    <hyperlink ref="C102" r:id="rId89" xr:uid="{3AD10C9E-4F6D-DE48-92F3-531A586520C6}"/>
+    <hyperlink ref="C103" r:id="rId90" xr:uid="{4FA217C0-A1F3-904E-8FEA-EA4941273A67}"/>
+    <hyperlink ref="C104" r:id="rId91" xr:uid="{A297BBC0-FA0D-2D46-9C49-3932193EF1D3}"/>
+    <hyperlink ref="C106" r:id="rId92" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance." xr:uid="{DCD751DE-E440-F346-B6FD-CBD072217214}"/>
+    <hyperlink ref="C107" r:id="rId93" xr:uid="{B2FD38B9-1E2B-8140-8291-F45734C98145}"/>
+    <hyperlink ref="C108" r:id="rId94" xr:uid="{C76888B3-18AC-9B48-9E2A-64A7DF0902B7}"/>
+    <hyperlink ref="C109" r:id="rId95" xr:uid="{18A79860-6C9E-A941-8D6C-360B9913E941}"/>
+    <hyperlink ref="C110" r:id="rId96" xr:uid="{C0DDFD68-CBC1-0F4A-AF40-ACF36BBC8453}"/>
+    <hyperlink ref="C111" r:id="rId97" xr:uid="{3E0BF737-E42E-C946-B32C-06882E0BA6FF}"/>
+    <hyperlink ref="C113" r:id="rId98" xr:uid="{862F9782-C57B-2848-A2D9-EB7B52FB7EC7}"/>
+    <hyperlink ref="C114" r:id="rId99" xr:uid="{230D7A6A-D2C5-C140-9A65-B1F407D22062}"/>
+    <hyperlink ref="C115" r:id="rId100" xr:uid="{BDC2BA28-4562-984E-8282-1126BF952EAF}"/>
+    <hyperlink ref="C116" r:id="rId101" xr:uid="{B53A5F28-6DED-3D47-8679-F78D3DDEFF01}"/>
+    <hyperlink ref="C117" r:id="rId102" xr:uid="{C57D0CC7-DA2F-0948-9BCE-F19C20C7D981}"/>
+    <hyperlink ref="C118" r:id="rId103" xr:uid="{117878E5-B8C8-254B-8ED6-014B4B7A8126}"/>
+    <hyperlink ref="C119" r:id="rId104" xr:uid="{B7CC0756-74F2-D54D-BDEE-9DA394DD7168}"/>
+    <hyperlink ref="C120" r:id="rId105" xr:uid="{837EF472-CCC2-CF47-A8A8-238E56F722CE}"/>
+    <hyperlink ref="C121" r:id="rId106" xr:uid="{3608F267-6AA0-624B-B243-7DDD317E9F08}"/>
+    <hyperlink ref="C122" r:id="rId107" xr:uid="{0B6123E6-0472-374B-ACA7-6914CD7918E8}"/>
+    <hyperlink ref="C123" r:id="rId108" xr:uid="{D3971CEB-C53E-B04B-9C32-1803182B5DC5}"/>
+    <hyperlink ref="C124" r:id="rId109" xr:uid="{7CF5013A-643E-1643-93A1-A2F1500D2A23}"/>
+    <hyperlink ref="C125" r:id="rId110" xr:uid="{2A6BE7E5-D818-6843-8C3E-99EA2BFE0FB2}"/>
+    <hyperlink ref="C126" r:id="rId111" xr:uid="{E718F544-96DF-A04E-8DFB-7639DA3EA57C}"/>
+    <hyperlink ref="C127" r:id="rId112" xr:uid="{B0C2F065-424A-7345-A864-346ECD98D749}"/>
+    <hyperlink ref="C128" r:id="rId113" xr:uid="{B4E26955-5C3F-804E-B19A-11260310AFB3}"/>
+    <hyperlink ref="C129" r:id="rId114" xr:uid="{6F299BB5-8E82-0240-A9A3-6829CE3ABCBF}"/>
+    <hyperlink ref="C130" r:id="rId115" xr:uid="{A42CA32F-2196-1840-A53D-E5073237C68D}"/>
+    <hyperlink ref="C131" r:id="rId116" xr:uid="{7ECF6EF4-962E-4642-9B1C-C3B70674793E}"/>
+    <hyperlink ref="C132" r:id="rId117" xr:uid="{2A109178-6B60-164E-9D25-42B3282137E3}"/>
+    <hyperlink ref="C133" r:id="rId118" xr:uid="{B3D38BD0-A6A1-8D41-8405-45E1BEEEEF06}"/>
+    <hyperlink ref="C134" r:id="rId119" xr:uid="{A1C26612-D040-2A41-A6A6-A8F2490C0A43}"/>
+    <hyperlink ref="C135" r:id="rId120" xr:uid="{C476E807-64CB-F44A-A23D-D21EBF6D001D}"/>
+    <hyperlink ref="C136" r:id="rId121" xr:uid="{9A414D55-D4A1-F147-9207-61B597D57136}"/>
+    <hyperlink ref="C105" r:id="rId122" xr:uid="{18B028A7-9B6F-D841-8548-924D70530779}"/>
+    <hyperlink ref="C112" r:id="rId123" xr:uid="{6D3E75EF-733F-7A4B-81C8-AEF6CB6335F0}"/>
+    <hyperlink ref="C139" r:id="rId124" xr:uid="{C9EB2682-BE0B-934B-B0B4-1DD1A1502647}"/>
+    <hyperlink ref="C140" r:id="rId125" xr:uid="{2992FED9-2B78-A342-92AA-E7C0F882FF17}"/>
+    <hyperlink ref="C141" r:id="rId126" xr:uid="{0084DA6F-EC84-BD48-BDA8-EBACA3BB3B3E}"/>
+    <hyperlink ref="C142" r:id="rId127" xr:uid="{30F2D415-4B2C-384C-8EAE-2CC71CB518E2}"/>
+    <hyperlink ref="C143" r:id="rId128" xr:uid="{40734C88-7C5B-9747-86D1-03463D9AD41A}"/>
+    <hyperlink ref="C144" r:id="rId129" xr:uid="{1040D22F-6729-104A-A229-CBDCED93024A}"/>
+    <hyperlink ref="C145" r:id="rId130" xr:uid="{E131FE61-FABF-8E4B-8EF0-F68379D8F836}"/>
+    <hyperlink ref="C146" r:id="rId131" xr:uid="{B2129272-1351-3745-883B-E6A7115450C8}"/>
+    <hyperlink ref="C147" r:id="rId132" xr:uid="{C8B2DEF0-2B69-C84E-8013-0B6F03FFC250}"/>
+    <hyperlink ref="C148" r:id="rId133" xr:uid="{536AC5CF-712F-BF48-94A9-D0E7DC013020}"/>
+    <hyperlink ref="C149" r:id="rId134" xr:uid="{2DABC9C7-43D4-1249-AF9B-5FA4552611CB}"/>
+    <hyperlink ref="C150" r:id="rId135" xr:uid="{DA62E73A-B495-F94A-BECE-D42E4CBF074A}"/>
+    <hyperlink ref="C151" r:id="rId136" xr:uid="{7F5E6966-850D-4F49-B2A5-678365713F28}"/>
+    <hyperlink ref="C152" r:id="rId137" xr:uid="{E9C4286D-8493-9A47-8B8C-09583FA72B70}"/>
+    <hyperlink ref="C153" r:id="rId138" xr:uid="{9EB0123C-84AE-1C4D-BA1A-C28CFB8EFB89}"/>
+    <hyperlink ref="C154" r:id="rId139" xr:uid="{9D11FED4-328F-674E-889D-EC781DD1D791}"/>
+    <hyperlink ref="C155" r:id="rId140" xr:uid="{48AE72DB-397B-464D-88AD-B8058ED29CC1}"/>
+    <hyperlink ref="C156" r:id="rId141" xr:uid="{152D50E9-7448-F542-AC66-05D0AE66664C}"/>
+    <hyperlink ref="C157" r:id="rId142" xr:uid="{34E6AF1B-5FB1-3A4B-8938-1DCF80831DC2}"/>
+    <hyperlink ref="C158" r:id="rId143" xr:uid="{E7F8B7CA-49F4-1946-91EE-E7582BE4E5DA}"/>
+    <hyperlink ref="C159" r:id="rId144" xr:uid="{3590A994-B7A2-C14D-9BF8-7AC8FE9E7F0F}"/>
+    <hyperlink ref="C160" r:id="rId145" xr:uid="{0AAA4B0C-4921-C34D-B41E-D702FA860892}"/>
+    <hyperlink ref="C161" r:id="rId146" xr:uid="{5973FCA4-AE32-5248-A6ED-2694367332F1}"/>
+    <hyperlink ref="C162" r:id="rId147" xr:uid="{4C0F816E-F043-0C47-BF16-1CDAD88D2FF1}"/>
+    <hyperlink ref="C163" r:id="rId148" xr:uid="{A8E4C654-D0BD-8945-9F5C-B09F7BC114BE}"/>
+    <hyperlink ref="C166" r:id="rId149" xr:uid="{E3825C15-10BB-E24F-B229-983F651DA942}"/>
+    <hyperlink ref="C167" r:id="rId150" xr:uid="{46ECFC31-388C-6241-8FFE-DED6F2FC794A}"/>
+    <hyperlink ref="C168" r:id="rId151" xr:uid="{589E024D-3FE1-1048-890C-88289733F233}"/>
+    <hyperlink ref="C169" r:id="rId152" xr:uid="{CDA28F7A-7FC5-F74D-B27E-A6E0161D41D5}"/>
+    <hyperlink ref="C170" r:id="rId153" xr:uid="{DA6A0D92-DCEB-DA4F-8BBA-10FCD092838F}"/>
+    <hyperlink ref="C171" r:id="rId154" xr:uid="{955769DB-3256-254B-90DE-E1E01B272F8A}"/>
+    <hyperlink ref="C172" r:id="rId155" xr:uid="{DED7AC9B-40D7-0545-9D6F-6CD4F5FFE4C6}"/>
+    <hyperlink ref="C173" r:id="rId156" xr:uid="{6947A4E1-B6AA-6D4F-A6D8-8FA74FD02887}"/>
+    <hyperlink ref="C174" r:id="rId157" xr:uid="{EABF2012-5A90-0C4E-86F6-FDB5FA7770BE}"/>
+    <hyperlink ref="C177" r:id="rId158" xr:uid="{7F44CFE0-9ED1-A44D-B9EF-CF87BEB644FC}"/>
+    <hyperlink ref="C178" r:id="rId159" xr:uid="{CF6E0CF6-7A93-D84A-9CE0-5BDD51767416}"/>
+    <hyperlink ref="C179" r:id="rId160" xr:uid="{EFF8F154-60B8-B84B-84CA-32756BD6430F}"/>
+    <hyperlink ref="C180" r:id="rId161" xr:uid="{C8A3094E-E11B-2543-B05E-1D07048B2EBA}"/>
+    <hyperlink ref="C181" r:id="rId162" xr:uid="{9961E5F5-B5C6-0C4D-A1D0-D04D2A5D7DFD}"/>
+    <hyperlink ref="C182" r:id="rId163" xr:uid="{44E289EC-47DD-D94D-88C1-CB2F59C6C16A}"/>
+    <hyperlink ref="C183" r:id="rId164" xr:uid="{4161FC70-DD6D-684B-898A-A4711596B2D5}"/>
+    <hyperlink ref="C184" r:id="rId165" xr:uid="{B9CBE387-8E9A-ED48-8310-CF7D34FA690C}"/>
+    <hyperlink ref="C185" r:id="rId166" xr:uid="{5398097B-24FF-9543-8F02-33CE2860F1F7}"/>
+    <hyperlink ref="C186" r:id="rId167" xr:uid="{3B1FC30B-30C8-7B48-AF94-A81FB513F24F}"/>
+    <hyperlink ref="C187" r:id="rId168" xr:uid="{32B750D0-D7F2-694D-AB9B-25AFAFAFF17F}"/>
+    <hyperlink ref="C188" r:id="rId169" xr:uid="{400689DD-8E95-024E-976B-AACD8ED4E1A6}"/>
+    <hyperlink ref="C189" r:id="rId170" xr:uid="{28753DDE-E047-5D40-A30B-1103BE6DA08F}"/>
+    <hyperlink ref="C190" r:id="rId171" xr:uid="{6C5AA6CB-3D93-0740-AEED-9E6C218CF6CB}"/>
+    <hyperlink ref="C191" r:id="rId172" xr:uid="{03EAA2B9-D8B8-D642-BF24-380596D26B2E}"/>
+    <hyperlink ref="C192" r:id="rId173" xr:uid="{8C1719B4-37CC-484E-BDCE-A4272C07F91B}"/>
+    <hyperlink ref="C193" r:id="rId174" xr:uid="{6C198DA2-BB98-F940-8EF6-2FC8B7AE577A}"/>
+    <hyperlink ref="C194" r:id="rId175" xr:uid="{AB0EA311-A446-D046-A0EC-290B42068328}"/>
+    <hyperlink ref="C195" r:id="rId176" xr:uid="{DB913045-B9F6-6549-AA09-22B0CC5FDD21}"/>
+    <hyperlink ref="C196" r:id="rId177" xr:uid="{806469FD-617A-7445-AAB5-FB2FD2ED24EA}"/>
+    <hyperlink ref="C197" r:id="rId178" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{1A10544E-58CF-D04D-9FAF-2FEC6DB2B5D4}"/>
+    <hyperlink ref="C198" r:id="rId179" xr:uid="{5A0B6645-89FD-E044-A706-9FB890274C3C}"/>
+    <hyperlink ref="C199" r:id="rId180" xr:uid="{B42A3009-E8EB-EE44-885F-6699C17A0E0B}"/>
+    <hyperlink ref="C200" r:id="rId181" xr:uid="{ED3E48AB-E25B-3744-B024-E97B2A319B46}"/>
+    <hyperlink ref="C201" r:id="rId182" xr:uid="{C75D20A3-CBAE-2649-A3EE-E49177CFA343}"/>
+    <hyperlink ref="C202" r:id="rId183" xr:uid="{3863CA1B-D43E-1144-91A9-17C2DCF52A64}"/>
+    <hyperlink ref="C203" r:id="rId184" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{E9AF434E-4CAA-5D49-8AD3-889CDE2913D9}"/>
+    <hyperlink ref="C204" r:id="rId185" xr:uid="{1A0568E5-3A11-7F47-8001-82B05D7C2339}"/>
+    <hyperlink ref="C205" r:id="rId186" xr:uid="{F62B8AE4-9C4F-9544-8861-CD733C12F79E}"/>
+    <hyperlink ref="C206" r:id="rId187" xr:uid="{0F6A542C-44C9-5A4C-90BF-BC8C239877D2}"/>
+    <hyperlink ref="C207" r:id="rId188" xr:uid="{3ED28203-B1B5-4E46-AAF3-779EDD4AC03F}"/>
+    <hyperlink ref="C208" r:id="rId189" xr:uid="{4338B305-B52F-5540-9B51-B938FC6803A2}"/>
+    <hyperlink ref="C209" r:id="rId190" xr:uid="{DDEEED0F-A939-1E4F-B2FA-AD391A4A2874}"/>
+    <hyperlink ref="C210" r:id="rId191" xr:uid="{C2F20589-AD81-654C-94E5-E5B6C9FE27F6}"/>
+    <hyperlink ref="C211" r:id="rId192" xr:uid="{BBEB9DAC-E4AE-C04F-AA15-6356AFC57FDE}"/>
+    <hyperlink ref="C214" r:id="rId193" xr:uid="{6316566D-A10A-F849-9F25-B9ED4DA12BC7}"/>
+    <hyperlink ref="C215" r:id="rId194" xr:uid="{9D4DD895-FBA6-C849-A5BF-3B30755BD9C9}"/>
+    <hyperlink ref="C216" r:id="rId195" xr:uid="{475996DA-632A-BE49-AEA1-D4189FD614A1}"/>
+    <hyperlink ref="C217" r:id="rId196" xr:uid="{88E0C858-8468-884F-BB71-F6F176BD5FC2}"/>
+    <hyperlink ref="C218" r:id="rId197" xr:uid="{C1C5C8D0-7A06-3D4A-A85A-AAACC1B418C9}"/>
+    <hyperlink ref="C219" r:id="rId198" xr:uid="{D525D4B1-2857-1543-8CD9-196728321203}"/>
+    <hyperlink ref="C220" r:id="rId199" xr:uid="{51E3AB9B-04B2-C041-A2B3-37E3EB18013A}"/>
+    <hyperlink ref="C221" r:id="rId200" xr:uid="{7F7F0C9A-57B9-314F-959A-B8ACAFA5FD13}"/>
+    <hyperlink ref="C222" r:id="rId201" xr:uid="{3B029785-83B4-6140-8B70-CD892CFC87F6}"/>
+    <hyperlink ref="C223" r:id="rId202" xr:uid="{B0A390E6-D860-9F4E-B021-68949FE712F3}"/>
+    <hyperlink ref="C224" r:id="rId203" xr:uid="{49E9953D-52F6-BF47-8AAA-8E456F55576B}"/>
+    <hyperlink ref="C225" r:id="rId204" xr:uid="{9B812470-F419-A54E-8365-06A9B8864A30}"/>
+    <hyperlink ref="C226" r:id="rId205" xr:uid="{B6FB4107-1933-6D45-9EF4-4474E06CBE9D}"/>
+    <hyperlink ref="C227" r:id="rId206" xr:uid="{0F7C1D92-7BCB-D14D-A658-9599984E04E4}"/>
+    <hyperlink ref="C228" r:id="rId207" xr:uid="{6810428F-0A78-964C-A8C8-E1CD2E7C405D}"/>
+    <hyperlink ref="C229" r:id="rId208" xr:uid="{B40209F2-0D6E-364F-8AF6-F1D182509314}"/>
+    <hyperlink ref="C230" r:id="rId209" xr:uid="{96C53FA9-9FD3-2D4F-B292-3C9DEDFA806E}"/>
+    <hyperlink ref="C231" r:id="rId210" xr:uid="{918B420D-3678-FD46-9463-595E8ACC39E1}"/>
+    <hyperlink ref="C232" r:id="rId211" xr:uid="{851A7153-3B54-0E4A-A0A0-FCEB091AFE70}"/>
+    <hyperlink ref="C233" r:id="rId212" xr:uid="{C03AE9F8-09AE-C640-81A7-033BB06FB6AD}"/>
+    <hyperlink ref="C234" r:id="rId213" xr:uid="{35140DEB-52D2-4342-88D2-22BA061E5B48}"/>
+    <hyperlink ref="C235" r:id="rId214" xr:uid="{9714BC0B-3373-934C-B7A1-599F74F4FB9D}"/>
+    <hyperlink ref="C238" r:id="rId215" xr:uid="{5CB435B2-7FD2-1D44-9872-22B6A1EDC02B}"/>
+    <hyperlink ref="C239" r:id="rId216" xr:uid="{722D1D95-896B-4642-BABD-31DEDD237B49}"/>
+    <hyperlink ref="C240" r:id="rId217" xr:uid="{D686D1DC-13D6-284C-B606-E087FAF47399}"/>
+    <hyperlink ref="C241" r:id="rId218" xr:uid="{D22C2394-C3CB-8F4F-A010-2B13C8C84D1A}"/>
+    <hyperlink ref="C242" r:id="rId219" xr:uid="{3AE2F800-B66F-1A41-893B-978F6875FDC8}"/>
+    <hyperlink ref="C243" r:id="rId220" xr:uid="{2C939BDE-5298-5541-837B-8C59D53A33C1}"/>
+    <hyperlink ref="C244" r:id="rId221" xr:uid="{691C9BD8-69D3-DA4B-AEB6-AF827B4ACA9F}"/>
+    <hyperlink ref="C245" r:id="rId222" xr:uid="{B6891E82-7C4D-424D-9219-3C9FD08E0053}"/>
+    <hyperlink ref="C246" r:id="rId223" xr:uid="{67A1AE98-62D2-644D-AC13-6CD76CF53CC0}"/>
+    <hyperlink ref="C247" r:id="rId224" xr:uid="{B59D4881-2A82-8F4D-B151-1E796C4923C8}"/>
+    <hyperlink ref="C248" r:id="rId225" xr:uid="{B3CBD023-5EFD-6048-9B3F-89F0C65CBBF5}"/>
+    <hyperlink ref="C249" r:id="rId226" xr:uid="{53EC42C4-22F7-0445-A0AC-7275A59A2672}"/>
+    <hyperlink ref="C250" r:id="rId227" xr:uid="{A29575F3-CB24-5B4B-9538-D5212B2DC28B}"/>
+    <hyperlink ref="C251" r:id="rId228" xr:uid="{353A44DD-9E30-8F48-8E2B-8DAA07550470}"/>
+    <hyperlink ref="C252" r:id="rId229" xr:uid="{32AC291D-95A5-BE49-88E0-02677BF39CAC}"/>
+    <hyperlink ref="C253" r:id="rId230" xr:uid="{A84F22FF-AD10-A546-8998-B066C0EB2D5A}"/>
+    <hyperlink ref="C254" r:id="rId231" xr:uid="{4C5CAF84-9B94-FC44-8C6C-B3CC7257C1DB}"/>
+    <hyperlink ref="C255" r:id="rId232" xr:uid="{5DA775E2-C516-3B47-8C82-3CEE7CC0BDF9}"/>
+    <hyperlink ref="C256" r:id="rId233" xr:uid="{00B6AE5C-EF3F-0747-A280-3BF055362B4F}"/>
+    <hyperlink ref="C257" r:id="rId234" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{BCBD0A7E-F3D0-E840-9375-AFD37C5CD41A}"/>
+    <hyperlink ref="C258" r:id="rId235" xr:uid="{47ABDDDB-F95F-8049-9FB3-1E71A7376DDE}"/>
+    <hyperlink ref="C259" r:id="rId236" xr:uid="{70BADFC9-7399-234D-99F6-4C5F02397C26}"/>
+    <hyperlink ref="C260" r:id="rId237" xr:uid="{63348580-70EF-EC47-BF49-8ECE9560D54E}"/>
+    <hyperlink ref="C261" r:id="rId238" xr:uid="{D5BD96B3-9EAB-1B47-AC87-5C47F6AD7F40}"/>
+    <hyperlink ref="C262" r:id="rId239" xr:uid="{74791141-3FB8-7540-B45B-9541AF0AE371}"/>
+    <hyperlink ref="C263" r:id="rId240" xr:uid="{88D53CD6-262A-7247-8E58-FE9FFF7ECC40}"/>
+    <hyperlink ref="C264" r:id="rId241" xr:uid="{4338A14D-4F7D-B943-A347-7F74EFCA0DB5}"/>
+    <hyperlink ref="C265" r:id="rId242" xr:uid="{6E0EF7A3-7341-284B-A0E3-4539B6EAFAF2}"/>
+    <hyperlink ref="C266" r:id="rId243" xr:uid="{D2D8D64F-E2D3-734E-AD45-3EFB9686555A}"/>
+    <hyperlink ref="C267" r:id="rId244" xr:uid="{04A2904A-73A0-7845-9868-2CCFE359AC68}"/>
+    <hyperlink ref="C268" r:id="rId245" xr:uid="{D3D35835-6BE3-4D41-AF6F-5FE442277A16}"/>
+    <hyperlink ref="C269" r:id="rId246" xr:uid="{F663D0FC-CFF0-BC4F-9D26-48C871A8E9FD}"/>
+    <hyperlink ref="C270" r:id="rId247" xr:uid="{DF544147-DA48-4041-A4E2-4A75106B771A}"/>
+    <hyperlink ref="C271" r:id="rId248" xr:uid="{50E4B716-239E-7946-843D-E8462591D128}"/>
+    <hyperlink ref="C272" r:id="rId249" xr:uid="{D368B3E5-7D12-FD48-AFF7-A4A614108940}"/>
+    <hyperlink ref="C275" r:id="rId250" xr:uid="{D5921FF1-FC1F-CA4B-A24E-AD69E1DEC14C}"/>
+    <hyperlink ref="C276" r:id="rId251" xr:uid="{C931D7E0-E032-7C4B-95F1-735D955FCB51}"/>
+    <hyperlink ref="C277" r:id="rId252" xr:uid="{5FBD4A8F-287C-2C46-9CAB-F7DBA67DEDDA}"/>
+    <hyperlink ref="C278" r:id="rId253" xr:uid="{12966DD6-41DD-A94B-8B2C-0AD7D2AD6FB0}"/>
+    <hyperlink ref="C279" r:id="rId254" xr:uid="{CF720C34-4554-2944-A818-020ABC9BF0F4}"/>
+    <hyperlink ref="C280" r:id="rId255" xr:uid="{75763F2A-16D7-DE43-8189-19623CE26370}"/>
+    <hyperlink ref="C281" r:id="rId256" xr:uid="{9263AA30-472A-0A4D-BADF-96D82BB9BFCC}"/>
+    <hyperlink ref="C282" r:id="rId257" xr:uid="{2EF025C3-75C8-564E-BA8B-708C32B0E602}"/>
+    <hyperlink ref="C283" r:id="rId258" xr:uid="{6BDFDCA9-3421-F24F-8EF2-A72742F0AC21}"/>
+    <hyperlink ref="C284" r:id="rId259" xr:uid="{D8447F99-5FF9-D544-99BB-E9969B4A38D7}"/>
+    <hyperlink ref="C285" r:id="rId260" xr:uid="{1DB7EFDA-6C7D-F546-9EE1-F61ED0F65209}"/>
+    <hyperlink ref="C286" r:id="rId261" xr:uid="{D1505609-27D1-784D-ACF6-AE9D0DA2E1B6}"/>
+    <hyperlink ref="C287" r:id="rId262" xr:uid="{6BFA7B45-17D0-4E49-85DA-23C7255A306D}"/>
+    <hyperlink ref="C288" r:id="rId263" xr:uid="{3324BA4A-30CA-5246-8C3C-6505A6987939}"/>
+    <hyperlink ref="C289" r:id="rId264" xr:uid="{894486AD-2B6D-5740-BCAF-0BA1AFF814B4}"/>
+    <hyperlink ref="C290" r:id="rId265" xr:uid="{C47B203B-8B5A-E740-8C86-0784AD28089E}"/>
+    <hyperlink ref="C291" r:id="rId266" xr:uid="{06DC2E54-7597-AE4D-ACDB-B8883A989A4F}"/>
+    <hyperlink ref="C292" r:id="rId267" xr:uid="{E3384259-7CA7-1C44-A66D-11346EE6742E}"/>
+    <hyperlink ref="C293" r:id="rId268" xr:uid="{A5B77769-38AF-3D47-A76B-311591B57D91}"/>
+    <hyperlink ref="C296" r:id="rId269" xr:uid="{9DB6976A-C646-1341-90E8-3A164521267A}"/>
+    <hyperlink ref="C297" r:id="rId270" xr:uid="{03C291F8-D19A-304B-9EF9-CF71A1F66E49}"/>
+    <hyperlink ref="C298" r:id="rId271" xr:uid="{7536415C-140B-9244-B0B2-23F3ED0B2D80}"/>
+    <hyperlink ref="C299" r:id="rId272" xr:uid="{7DBDA456-8AF6-DD43-9764-17D3959B8E8F}"/>
+    <hyperlink ref="C300" r:id="rId273" xr:uid="{BFC149AB-C15A-B648-9F6A-ECD3890B1918}"/>
+    <hyperlink ref="C301" r:id="rId274" xr:uid="{0482240B-FEE9-F746-8980-52BCB7BBB56E}"/>
+    <hyperlink ref="C302" r:id="rId275" xr:uid="{86D1231A-E7C8-4B45-99ED-2DB0EF71E190}"/>
+    <hyperlink ref="C303" r:id="rId276" xr:uid="{20B7CE89-CB37-0040-989F-C8D1BE2B8782}"/>
+    <hyperlink ref="C304" r:id="rId277" xr:uid="{4C8412C9-A47B-9244-A18B-741516BD1054}"/>
+    <hyperlink ref="C305" r:id="rId278" xr:uid="{511761D9-31CE-0B43-AFFD-C011C27ACC52}"/>
+    <hyperlink ref="C306" r:id="rId279" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{6905F997-D048-1049-BA27-C48756603D1E}"/>
+    <hyperlink ref="C307" r:id="rId280" xr:uid="{E657AA82-7CFE-DB42-B20F-F63D8C25EAB6}"/>
+    <hyperlink ref="C308" r:id="rId281" xr:uid="{3E505033-58F3-8F4E-AB82-E12DBC226AEA}"/>
+    <hyperlink ref="C309" r:id="rId282" xr:uid="{749599E5-4972-7343-B13B-87E26F837470}"/>
+    <hyperlink ref="C310" r:id="rId283" xr:uid="{12AA88DC-22AB-5A49-B28C-F04C8E35A215}"/>
+    <hyperlink ref="C311" r:id="rId284" xr:uid="{5751F0A7-7D9D-4148-820B-5B9659DFE34F}"/>
+    <hyperlink ref="C312" r:id="rId285" xr:uid="{4CA2DBEE-B161-B84D-B3A9-B8BC1B598AF2}"/>
+    <hyperlink ref="C313" r:id="rId286" xr:uid="{A9C1E578-6594-954C-8785-8902E605FC7A}"/>
+    <hyperlink ref="C314" r:id="rId287" xr:uid="{3D45E9B8-6671-A747-8C18-51CF8883170A}"/>
+    <hyperlink ref="C315" r:id="rId288" xr:uid="{4F5EF748-8CD4-0F47-90CE-3C93755BF63D}"/>
+    <hyperlink ref="C316" r:id="rId289" xr:uid="{44053C08-5050-C84B-B016-069B1EF9A43D}"/>
+    <hyperlink ref="C317" r:id="rId290" xr:uid="{ABF38928-736B-1A49-8B8A-1DCA5AAECB2B}"/>
+    <hyperlink ref="C318" r:id="rId291" xr:uid="{52651FAF-F3DC-E949-8AF8-998B9724B7D1}"/>
+    <hyperlink ref="C319" r:id="rId292" xr:uid="{91C6CCEF-3FF7-2C42-B5A0-8F4A403ED198}"/>
+    <hyperlink ref="C320" r:id="rId293" xr:uid="{15C8AF08-1A79-F949-9BE7-DD240CBD9861}"/>
+    <hyperlink ref="C321" r:id="rId294" xr:uid="{1904F984-5B22-8D46-BC33-3073B390E8F9}"/>
+    <hyperlink ref="C322" r:id="rId295" xr:uid="{A8BFB3A4-426B-E646-BCF0-FE19C8CD07A9}"/>
+    <hyperlink ref="C323" r:id="rId296" xr:uid="{FBBA29BB-885B-744A-A644-58EDCA7B140A}"/>
+    <hyperlink ref="C324" r:id="rId297" xr:uid="{75411687-6884-AC42-8B4A-1348C4837365}"/>
+    <hyperlink ref="C325" r:id="rId298" xr:uid="{A89ED8DF-F678-FE43-808C-C190721379BF}"/>
+    <hyperlink ref="C326" r:id="rId299" xr:uid="{1516834D-F3B2-1743-8811-263E11BBDEF8}"/>
+    <hyperlink ref="C327" r:id="rId300" xr:uid="{1659AB91-08CA-E44D-988D-E9D9A746D406}"/>
+    <hyperlink ref="C328" r:id="rId301" xr:uid="{E844BC1D-9713-9F4D-B0A4-1124A9952D14}"/>
+    <hyperlink ref="C329" r:id="rId302" xr:uid="{DCE2AAEF-8D8E-1843-BFE9-E9B7E13854EB}"/>
+    <hyperlink ref="C330" r:id="rId303" xr:uid="{836B3BF0-7711-7D41-9E72-914C1871397F}"/>
+    <hyperlink ref="C331" r:id="rId304" xr:uid="{F450CF9B-CA59-1443-8163-13F1121DCF12}"/>
+    <hyperlink ref="C332" r:id="rId305" xr:uid="{1539C3E8-4854-3C4F-A7B3-55BF931F1E2A}"/>
+    <hyperlink ref="C333" r:id="rId306" xr:uid="{04F1FC5F-5DA1-0144-962D-B38C1C41F0F4}"/>
+    <hyperlink ref="C336" r:id="rId307" xr:uid="{B21618F4-70E2-C549-80B7-7CF915679E0A}"/>
+    <hyperlink ref="C337" r:id="rId308" xr:uid="{EEDFBF11-C1E4-0847-9D56-94A72D97AEE7}"/>
+    <hyperlink ref="C338" r:id="rId309" xr:uid="{F5C0EDF1-7EAC-8849-8D27-C3389913BFC6}"/>
+    <hyperlink ref="C339" r:id="rId310" xr:uid="{50175B29-124F-4E4E-8E98-961BD3320359}"/>
+    <hyperlink ref="C340" r:id="rId311" xr:uid="{1BE23822-8512-014F-9154-F6EDA4FC8428}"/>
+    <hyperlink ref="C341" r:id="rId312" xr:uid="{38EC228E-ABFF-3542-9CFB-3DDFC628E9D0}"/>
+    <hyperlink ref="C342" r:id="rId313" xr:uid="{73F240F8-C469-454E-BA5C-CFF2F7A7A5F6}"/>
+    <hyperlink ref="C343" r:id="rId314" xr:uid="{3BBD1BAC-68C7-A94A-9063-AF62B5C837FD}"/>
+    <hyperlink ref="C344" r:id="rId315" xr:uid="{F9751D9B-2689-E24B-9FC3-CA32FE888708}"/>
+    <hyperlink ref="C345" r:id="rId316" xr:uid="{73C61D6A-D97C-B944-8B27-BB91564AB0D7}"/>
+    <hyperlink ref="C346" r:id="rId317" xr:uid="{936E077C-C016-A04F-895A-782D6D9D9433}"/>
+    <hyperlink ref="C347" r:id="rId318" xr:uid="{5454A2A1-6607-BE48-9215-CB8965EC3568}"/>
+    <hyperlink ref="C348" r:id="rId319" xr:uid="{FC1EAA10-F7ED-6B42-A79B-3D8B44E2C8B3}"/>
+    <hyperlink ref="C349" r:id="rId320" xr:uid="{FDB7F712-4A42-1048-8929-A1E752B07C6A}"/>
+    <hyperlink ref="C350" r:id="rId321" xr:uid="{AF3ACA60-0B0E-E146-B51F-A2CD05EB6549}"/>
+    <hyperlink ref="C351" r:id="rId322" xr:uid="{BB63E040-7A1A-E046-9BDD-9CBD1DA89DE9}"/>
+    <hyperlink ref="C352" r:id="rId323" xr:uid="{9AF8FD93-CCC9-D540-AE9A-00583F309649}"/>
+    <hyperlink ref="C353" r:id="rId324" xr:uid="{66A746A0-71FE-E546-92B7-D1C3D582E067}"/>
+    <hyperlink ref="C357" r:id="rId325" xr:uid="{BD79CCE1-5315-3944-9F9B-618615EC4583}"/>
+    <hyperlink ref="C358" r:id="rId326" xr:uid="{A5068A51-C961-6847-BB27-40A850B6D393}"/>
+    <hyperlink ref="C359" r:id="rId327" xr:uid="{6B8D36F0-E796-B944-A456-E8A9E2EE0BDB}"/>
+    <hyperlink ref="C360" r:id="rId328" xr:uid="{776652B7-2C11-4641-BF6A-EABEEB9B55AB}"/>
+    <hyperlink ref="C361" r:id="rId329" xr:uid="{95C6B35D-712A-2343-B790-236B55C5EC49}"/>
+    <hyperlink ref="C362" r:id="rId330" xr:uid="{4ED53872-1FE9-F140-AA35-F228F762880B}"/>
+    <hyperlink ref="C363" r:id="rId331" xr:uid="{6D5E6A28-85AA-BF4C-B2BD-9378D6E28EC7}"/>
+    <hyperlink ref="C364" r:id="rId332" xr:uid="{BCAD1ECB-15EE-CF49-878E-AA682DE3AC22}"/>
+    <hyperlink ref="C365" r:id="rId333" xr:uid="{C85468B5-25E9-E446-808E-72CFE911F0C2}"/>
+    <hyperlink ref="C366" r:id="rId334" xr:uid="{9503AECA-1A6A-9640-A04C-4CEAA2304448}"/>
+    <hyperlink ref="C367" r:id="rId335" xr:uid="{74211516-06B0-AA45-845B-52C8202751DA}"/>
+    <hyperlink ref="C368" r:id="rId336" xr:uid="{02C696BC-4B91-9444-900F-9CD68E409ABC}"/>
+    <hyperlink ref="C369" r:id="rId337" xr:uid="{04646C45-4118-374C-839D-94D31D534FAC}"/>
+    <hyperlink ref="C370" r:id="rId338" xr:uid="{F90BCCAE-8596-FC4D-BDD7-774392C596DF}"/>
+    <hyperlink ref="C371" r:id="rId339" xr:uid="{65230925-36EC-8A4B-8E46-6350B9BC0F95}"/>
+    <hyperlink ref="C372" r:id="rId340" xr:uid="{E91B8177-0C7A-1F40-BD34-4CC60F03B84F}"/>
+    <hyperlink ref="C373" r:id="rId341" xr:uid="{E8CBFD60-7335-0B4D-9FF5-99B4A8DC551D}"/>
+    <hyperlink ref="C374" r:id="rId342" xr:uid="{A35F55D4-9B87-C745-94DB-E7D820193C30}"/>
+    <hyperlink ref="C375" r:id="rId343" xr:uid="{6461A29F-D404-334F-B13F-296B4CA5E8A4}"/>
+    <hyperlink ref="C376" r:id="rId344" xr:uid="{FA9B4BE7-85CC-B24F-9461-5E9B42DDD824}"/>
+    <hyperlink ref="C377" r:id="rId345" xr:uid="{A75ACEA2-CDF6-A147-8540-A6DF55B15F45}"/>
+    <hyperlink ref="C378" r:id="rId346" xr:uid="{62FF87E2-E658-AB4D-AC57-7BCF9D49516E}"/>
+    <hyperlink ref="C379" r:id="rId347" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{269338A6-5145-6944-9F7F-BD2A86DFA308}"/>
+    <hyperlink ref="C380" r:id="rId348" xr:uid="{8F583049-CE8D-CD42-88CD-CF3857942670}"/>
+    <hyperlink ref="C381" r:id="rId349" xr:uid="{EE2348AD-E296-894A-B5AE-5884A3C5E419}"/>
+    <hyperlink ref="C382" r:id="rId350" xr:uid="{6EACB34E-B32E-8F43-8055-2406F7417A7E}"/>
+    <hyperlink ref="C383" r:id="rId351" xr:uid="{2446F10A-B762-B64C-97B2-6131A0BECC1F}"/>
+    <hyperlink ref="C384" r:id="rId352" xr:uid="{6FDFCC53-17A6-7244-88A7-49406D7C9200}"/>
+    <hyperlink ref="C385" r:id="rId353" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
+    <hyperlink ref="C386" r:id="rId354" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
+    <hyperlink ref="C387" r:id="rId355" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
+    <hyperlink ref="C388" r:id="rId356" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
+    <hyperlink ref="C389" r:id="rId357" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
+    <hyperlink ref="C390" r:id="rId358" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
+    <hyperlink ref="C391" r:id="rId359" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
+    <hyperlink ref="C392" r:id="rId360" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
+    <hyperlink ref="C393" r:id="rId361" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
+    <hyperlink ref="C394" r:id="rId362" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
+    <hyperlink ref="C396" r:id="rId363" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
+    <hyperlink ref="C395" r:id="rId364" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
+    <hyperlink ref="C397" r:id="rId365" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
+    <hyperlink ref="C398" r:id="rId366" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
+    <hyperlink ref="C399" r:id="rId367" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
+    <hyperlink ref="C402" r:id="rId368" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
+    <hyperlink ref="C403" r:id="rId369" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
+    <hyperlink ref="C404" r:id="rId370" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
+    <hyperlink ref="C405" r:id="rId371" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
+    <hyperlink ref="C406" r:id="rId372" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
+    <hyperlink ref="C407" r:id="rId373" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
+    <hyperlink ref="C410" r:id="rId374" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
+    <hyperlink ref="C411" r:id="rId375" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
+    <hyperlink ref="C412" r:id="rId376" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
+    <hyperlink ref="C413" r:id="rId377" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
+    <hyperlink ref="C414" r:id="rId378" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
+    <hyperlink ref="C415" r:id="rId379" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
+    <hyperlink ref="C416" r:id="rId380" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
+    <hyperlink ref="C417" r:id="rId381" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
+    <hyperlink ref="C418" r:id="rId382" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
+    <hyperlink ref="C419" r:id="rId383" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
+    <hyperlink ref="C420" r:id="rId384" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
+    <hyperlink ref="C421" r:id="rId385" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
+    <hyperlink ref="C422" r:id="rId386" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
+    <hyperlink ref="C423" r:id="rId387" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
+    <hyperlink ref="C424" r:id="rId388" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
+    <hyperlink ref="C425" r:id="rId389" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
+    <hyperlink ref="C426" r:id="rId390" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
+    <hyperlink ref="C427" r:id="rId391" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
+    <hyperlink ref="C428" r:id="rId392" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
+    <hyperlink ref="C429" r:id="rId393" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
+    <hyperlink ref="C430" r:id="rId394" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
+    <hyperlink ref="C431" r:id="rId395" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
+    <hyperlink ref="C432" r:id="rId396" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
+    <hyperlink ref="C433" r:id="rId397" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
+    <hyperlink ref="C434" r:id="rId398" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
+    <hyperlink ref="C435" r:id="rId399" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
+    <hyperlink ref="C436" r:id="rId400" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
+    <hyperlink ref="C437" r:id="rId401" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
+    <hyperlink ref="C438" r:id="rId402" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
+    <hyperlink ref="C439" r:id="rId403" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
+    <hyperlink ref="C440" r:id="rId404" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
+    <hyperlink ref="C441" r:id="rId405" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
+    <hyperlink ref="C442" r:id="rId406" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
+    <hyperlink ref="C443" r:id="rId407" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
+    <hyperlink ref="C444" r:id="rId408" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
+    <hyperlink ref="C445" r:id="rId409" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
+    <hyperlink ref="C446" r:id="rId410" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
+    <hyperlink ref="C447" r:id="rId411" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
+    <hyperlink ref="C448" r:id="rId412" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
+    <hyperlink ref="C449" r:id="rId413" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
+    <hyperlink ref="C451" r:id="rId414" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
+    <hyperlink ref="C450" r:id="rId415" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
+    <hyperlink ref="C452" r:id="rId416" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
+    <hyperlink ref="C453" r:id="rId417" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
+    <hyperlink ref="C454" r:id="rId418" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
+    <hyperlink ref="C455" r:id="rId419" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
+    <hyperlink ref="C456" r:id="rId420" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
+    <hyperlink ref="C457" r:id="rId421" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
+    <hyperlink ref="C458" r:id="rId422" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
+    <hyperlink ref="C459" r:id="rId423" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
+    <hyperlink ref="C460" r:id="rId424" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
+    <hyperlink ref="C461" r:id="rId425" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
+    <hyperlink ref="C462" r:id="rId426" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
+    <hyperlink ref="C469" r:id="rId427" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
+    <hyperlink ref="C468" r:id="rId428" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
+    <hyperlink ref="C467" r:id="rId429" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
+    <hyperlink ref="C466" r:id="rId430" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
+    <hyperlink ref="C465" r:id="rId431" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
+    <hyperlink ref="C464" r:id="rId432" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
+    <hyperlink ref="C463" r:id="rId433" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
+    <hyperlink ref="C472" r:id="rId434" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
+    <hyperlink ref="C473" r:id="rId435" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
+    <hyperlink ref="C474" r:id="rId436" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
+    <hyperlink ref="C475" r:id="rId437" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
+    <hyperlink ref="C476" r:id="rId438" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
+    <hyperlink ref="C477" r:id="rId439" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
+    <hyperlink ref="C478" r:id="rId440" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
+    <hyperlink ref="C481" r:id="rId441" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
+    <hyperlink ref="C479" r:id="rId442" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
+    <hyperlink ref="C480" r:id="rId443" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
+    <hyperlink ref="C356" r:id="rId444" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
+    <hyperlink ref="C2" r:id="rId445" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
+    <hyperlink ref="C88" r:id="rId446" display="Write a program tofind the smallest window that contains all characters of string itself." xr:uid="{8E3D4BDF-9F8F-0542-BFD8-C3CE3BF396E6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId447"/>

</xml_diff>

<commit_message>
Added dates in excel sheet
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF94916-D2F0-4427-B9D3-4477362C2113}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050422A9-443E-4C72-89EC-F554DE0656F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="470">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1432,6 +1432,9 @@
   </si>
   <si>
     <t>Write a program tofind the smallest window that contains all characters of string itself. (Please see pep coding soln in youtube for clarity)</t>
+  </si>
+  <si>
+    <t>Date to be completed by</t>
   </si>
 </sst>
 </file>
@@ -1568,7 +1571,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1607,6 +1610,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -1924,10 +1928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:D481"/>
+  <dimension ref="A1:E481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="E142" sqref="E142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1935,30 +1939,33 @@
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="28.5" customWidth="1"/>
     <col min="3" max="3" width="159.8984375" customWidth="1"/>
-    <col min="4" max="4" width="42.3984375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="9" customWidth="1"/>
     <col min="5" max="5" width="23.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24.6">
+    <row r="1" spans="1:5" ht="24.6">
       <c r="A1" s="17" t="s">
         <v>459</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="17"/>
       <c r="C2" s="8" t="s">
         <v>457</v>
       </c>
       <c r="D2" s="12"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="17"/>
       <c r="D3" s="12"/>
     </row>
-    <row r="4" spans="1:4" ht="21">
+    <row r="4" spans="1:5" ht="21">
       <c r="A4" s="17"/>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -1970,7 +1977,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="B5" s="15"/>
       <c r="C5" t="s">
         <v>461</v>
@@ -1979,7 +1986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="21">
+    <row r="6" spans="1:5" ht="21">
       <c r="A6" s="12">
         <v>1</v>
       </c>
@@ -1993,7 +2000,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="21">
+    <row r="7" spans="1:5" ht="21">
       <c r="A7" s="12">
         <v>2</v>
       </c>
@@ -2007,7 +2014,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="21">
+    <row r="8" spans="1:5" ht="21">
       <c r="A8" s="12">
         <v>3</v>
       </c>
@@ -2021,7 +2028,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="21">
+    <row r="9" spans="1:5" ht="21">
       <c r="A9" s="12">
         <v>4</v>
       </c>
@@ -2035,7 +2042,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="21">
+    <row r="10" spans="1:5" ht="21">
       <c r="A10" s="12">
         <v>5</v>
       </c>
@@ -2049,7 +2056,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="21">
+    <row r="11" spans="1:5" ht="21">
       <c r="A11" s="12">
         <v>6</v>
       </c>
@@ -2063,7 +2070,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="21">
+    <row r="12" spans="1:5" ht="21">
       <c r="A12" s="12">
         <v>7</v>
       </c>
@@ -2077,7 +2084,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="21">
+    <row r="13" spans="1:5" ht="21">
       <c r="A13" s="12">
         <v>8</v>
       </c>
@@ -2091,7 +2098,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="21">
+    <row r="14" spans="1:5" ht="21">
       <c r="A14" s="15">
         <v>9</v>
       </c>
@@ -2105,7 +2112,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="21">
+    <row r="15" spans="1:5" ht="21">
       <c r="A15" s="15">
         <v>10</v>
       </c>
@@ -2119,7 +2126,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="21">
+    <row r="16" spans="1:5" ht="21">
       <c r="A16" s="12">
         <v>11</v>
       </c>
@@ -2990,7 +2997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="21">
+    <row r="81" spans="1:5" ht="21">
       <c r="A81" s="12">
         <v>72</v>
       </c>
@@ -3004,7 +3011,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="21">
+    <row r="82" spans="1:5" ht="21">
       <c r="A82" s="12">
         <v>73</v>
       </c>
@@ -3018,7 +3025,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="21">
+    <row r="83" spans="1:5" ht="21">
       <c r="A83" s="15">
         <v>74</v>
       </c>
@@ -3032,7 +3039,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="21">
+    <row r="84" spans="1:5" ht="21">
       <c r="A84" s="12">
         <v>75</v>
       </c>
@@ -3046,7 +3053,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="21">
+    <row r="85" spans="1:5" ht="21">
       <c r="A85" s="15">
         <v>76</v>
       </c>
@@ -3060,7 +3067,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="21">
+    <row r="86" spans="1:5" ht="21">
       <c r="A86" s="15">
         <v>77</v>
       </c>
@@ -3074,7 +3081,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="21">
+    <row r="87" spans="1:5" ht="21">
       <c r="A87" s="16">
         <v>78</v>
       </c>
@@ -3088,7 +3095,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="21">
+    <row r="88" spans="1:5" ht="21">
       <c r="A88" s="16">
         <v>79</v>
       </c>
@@ -3102,7 +3109,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="21">
+    <row r="89" spans="1:5" ht="21">
       <c r="A89" s="16">
         <v>80</v>
       </c>
@@ -3116,7 +3123,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="21">
+    <row r="90" spans="1:5" ht="21">
       <c r="A90" s="16">
         <v>81</v>
       </c>
@@ -3130,7 +3137,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="21">
+    <row r="91" spans="1:5" ht="21">
       <c r="A91" s="16">
         <v>82</v>
       </c>
@@ -3143,8 +3150,11 @@
       <c r="D91" s="11" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" ht="21">
+      <c r="E91" s="18">
+        <v>44323</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="21">
       <c r="A92">
         <v>83</v>
       </c>
@@ -3157,8 +3167,11 @@
       <c r="D92" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" ht="21">
+      <c r="E92" s="18">
+        <v>44324</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="21">
       <c r="A93">
         <v>84</v>
       </c>
@@ -3171,8 +3184,11 @@
       <c r="D93" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" ht="21">
+      <c r="E93" s="18">
+        <v>44324</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="21">
       <c r="A94">
         <v>85</v>
       </c>
@@ -3185,8 +3201,11 @@
       <c r="D94" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" ht="21">
+      <c r="E94" s="18">
+        <v>44324</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="21">
       <c r="A95">
         <v>86</v>
       </c>
@@ -3199,8 +3218,11 @@
       <c r="D95" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" ht="21">
+      <c r="E95" s="18">
+        <v>44325</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="21">
       <c r="A96">
         <v>87</v>
       </c>
@@ -3213,8 +3235,11 @@
       <c r="D96" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" ht="21">
+      <c r="E96" s="18">
+        <v>44325</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="21">
       <c r="A97">
         <v>88</v>
       </c>
@@ -3227,8 +3252,11 @@
       <c r="D97" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" ht="21">
+      <c r="E97" s="18">
+        <v>44325</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="21">
       <c r="A98">
         <v>89</v>
       </c>
@@ -3241,13 +3269,16 @@
       <c r="D98" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" ht="21">
+      <c r="E98" s="18">
+        <v>44326</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="21">
       <c r="B100" s="6"/>
       <c r="C100" s="5"/>
       <c r="D100" s="10"/>
     </row>
-    <row r="101" spans="1:4" ht="21">
+    <row r="101" spans="1:5" ht="21">
       <c r="A101">
         <v>90</v>
       </c>
@@ -3261,7 +3292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="21">
+    <row r="102" spans="1:5" ht="21">
       <c r="A102">
         <v>91</v>
       </c>
@@ -3275,7 +3306,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="21">
+    <row r="103" spans="1:5" ht="21">
       <c r="A103">
         <v>92</v>
       </c>
@@ -3289,7 +3320,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="21">
+    <row r="104" spans="1:5" ht="21">
       <c r="A104">
         <v>93</v>
       </c>
@@ -3303,7 +3334,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="21">
+    <row r="105" spans="1:5" ht="21">
       <c r="A105">
         <v>94</v>
       </c>
@@ -3317,7 +3348,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="21">
+    <row r="106" spans="1:5" ht="21">
       <c r="A106">
         <v>95</v>
       </c>
@@ -3331,7 +3362,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="21">
+    <row r="107" spans="1:5" ht="21">
       <c r="A107">
         <v>96</v>
       </c>
@@ -3345,7 +3376,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="21">
+    <row r="108" spans="1:5" ht="21">
       <c r="A108">
         <v>97</v>
       </c>
@@ -3359,7 +3390,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="21">
+    <row r="109" spans="1:5" ht="21">
       <c r="A109">
         <v>98</v>
       </c>
@@ -3373,7 +3404,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="21">
+    <row r="110" spans="1:5" ht="21">
       <c r="A110">
         <v>99</v>
       </c>
@@ -3387,7 +3418,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="21">
+    <row r="111" spans="1:5" ht="21">
       <c r="A111">
         <v>100</v>
       </c>
@@ -3401,7 +3432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="21">
+    <row r="112" spans="1:5" ht="21">
       <c r="A112">
         <v>101</v>
       </c>
@@ -3639,7 +3670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="21">
+    <row r="129" spans="1:5" ht="21">
       <c r="A129">
         <v>118</v>
       </c>
@@ -3653,7 +3684,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="21">
+    <row r="130" spans="1:5" ht="21">
       <c r="A130">
         <v>119</v>
       </c>
@@ -3667,7 +3698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="21">
+    <row r="131" spans="1:5" ht="21">
       <c r="A131">
         <v>120</v>
       </c>
@@ -3681,7 +3712,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="21">
+    <row r="132" spans="1:5" ht="21">
       <c r="A132">
         <v>121</v>
       </c>
@@ -3695,7 +3726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="21">
+    <row r="133" spans="1:5" ht="21">
       <c r="A133">
         <v>122</v>
       </c>
@@ -3709,7 +3740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="21">
+    <row r="134" spans="1:5" ht="21">
       <c r="A134">
         <v>123</v>
       </c>
@@ -3723,7 +3754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="21">
+    <row r="135" spans="1:5" ht="21">
       <c r="A135">
         <v>124</v>
       </c>
@@ -3737,7 +3768,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="21">
+    <row r="136" spans="1:5" ht="21">
       <c r="A136">
         <v>125</v>
       </c>
@@ -3751,11 +3782,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="21">
+    <row r="138" spans="1:5" ht="21">
       <c r="C138" s="5"/>
       <c r="D138" s="10"/>
     </row>
-    <row r="139" spans="1:4" ht="21">
+    <row r="139" spans="1:5" ht="21">
       <c r="A139">
         <v>126</v>
       </c>
@@ -3768,8 +3799,11 @@
       <c r="D139" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" ht="21">
+      <c r="E139" s="18">
+        <v>44326</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="21">
       <c r="A140">
         <v>127</v>
       </c>
@@ -3782,8 +3816,11 @@
       <c r="D140" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" ht="21">
+      <c r="E140" s="18">
+        <v>44326</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="21">
       <c r="A141">
         <v>128</v>
       </c>
@@ -3796,8 +3833,11 @@
       <c r="D141" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" ht="21">
+      <c r="E141" s="18">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="21">
       <c r="A142">
         <v>129</v>
       </c>
@@ -3810,8 +3850,11 @@
       <c r="D142" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" ht="21">
+      <c r="E142" s="18">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="21">
       <c r="A143">
         <v>130</v>
       </c>
@@ -3825,7 +3868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="21">
+    <row r="144" spans="1:5" ht="21">
       <c r="A144">
         <v>131</v>
       </c>

</xml_diff>

<commit_message>
Some changes in problem 53,83
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050422A9-443E-4C72-89EC-F554DE0656F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06029CBB-3EA2-4F03-A94C-DFD0A2E98038}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1607,10 +1607,10 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -1930,8 +1930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:E481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="E142" sqref="E142"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1944,7 +1944,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24.6">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>459</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1955,18 +1955,18 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="17"/>
+      <c r="A2" s="18"/>
       <c r="C2" s="8" t="s">
         <v>457</v>
       </c>
       <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="17"/>
+      <c r="A3" s="18"/>
       <c r="D3" s="12"/>
     </row>
     <row r="4" spans="1:5" ht="21">
-      <c r="A4" s="17"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -3150,7 +3150,7 @@
       <c r="D91" s="11" t="s">
         <v>458</v>
       </c>
-      <c r="E91" s="18">
+      <c r="E91" s="17">
         <v>44323</v>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       <c r="D92" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E92" s="18">
+      <c r="E92" s="17">
         <v>44324</v>
       </c>
     </row>
@@ -3184,7 +3184,7 @@
       <c r="D93" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E93" s="18">
+      <c r="E93" s="17">
         <v>44324</v>
       </c>
     </row>
@@ -3201,7 +3201,7 @@
       <c r="D94" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E94" s="18">
+      <c r="E94" s="17">
         <v>44324</v>
       </c>
     </row>
@@ -3218,7 +3218,7 @@
       <c r="D95" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E95" s="18">
+      <c r="E95" s="17">
         <v>44325</v>
       </c>
     </row>
@@ -3235,7 +3235,7 @@
       <c r="D96" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E96" s="18">
+      <c r="E96" s="17">
         <v>44325</v>
       </c>
     </row>
@@ -3252,7 +3252,7 @@
       <c r="D97" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E97" s="18">
+      <c r="E97" s="17">
         <v>44325</v>
       </c>
     </row>
@@ -3269,7 +3269,7 @@
       <c r="D98" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E98" s="18">
+      <c r="E98" s="17">
         <v>44326</v>
       </c>
     </row>
@@ -3799,7 +3799,7 @@
       <c r="D139" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E139" s="18">
+      <c r="E139" s="17">
         <v>44326</v>
       </c>
     </row>
@@ -3816,7 +3816,7 @@
       <c r="D140" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E140" s="18">
+      <c r="E140" s="17">
         <v>44326</v>
       </c>
     </row>
@@ -3833,7 +3833,7 @@
       <c r="D141" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E141" s="18">
+      <c r="E141" s="17">
         <v>44327</v>
       </c>
     </row>
@@ -3850,7 +3850,7 @@
       <c r="D142" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E142" s="18">
+      <c r="E142" s="17">
         <v>44327</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove Consecutive Characters added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2949C426-42AF-4317-B772-0E1BA202FA5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9246324C-021C-4CDB-877D-1D8CAE1D6F06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1617,10 +1617,10 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -1941,7 +1941,7 @@
   <dimension ref="A1:E481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A84" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="E92" sqref="E92"/>
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1954,7 +1954,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24.6">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>459</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1965,18 +1965,18 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="18"/>
+      <c r="A2" s="19"/>
       <c r="C2" s="8" t="s">
         <v>457</v>
       </c>
       <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="18"/>
+      <c r="A3" s="19"/>
       <c r="D3" s="12"/>
     </row>
     <row r="4" spans="1:5" ht="21">
-      <c r="A4" s="18"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -3163,7 +3163,7 @@
       <c r="E91" s="17"/>
     </row>
     <row r="92" spans="1:5" ht="21">
-      <c r="A92" s="19">
+      <c r="A92" s="18">
         <v>83</v>
       </c>
       <c r="B92" s="3" t="s">
@@ -3180,7 +3180,7 @@
       </c>
     </row>
     <row r="93" spans="1:5" ht="21">
-      <c r="A93">
+      <c r="A93" s="12">
         <v>84</v>
       </c>
       <c r="B93" s="3" t="s">
@@ -3189,8 +3189,8 @@
       <c r="C93" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D93" s="10" t="s">
-        <v>4</v>
+      <c r="D93" s="11" t="s">
+        <v>458</v>
       </c>
       <c r="E93" s="17"/>
     </row>

</xml_diff>

<commit_message>
Wildcard String Matching addded
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9246324C-021C-4CDB-877D-1D8CAE1D6F06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9892DFA-2FD1-4CFF-A477-F6F9E1ABED07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1529,7 +1529,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1554,12 +1554,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1580,7 +1574,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1615,9 +1609,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1940,8 +1933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:E481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1954,7 +1947,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24.6">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>459</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1965,18 +1958,18 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="19"/>
+      <c r="A2" s="18"/>
       <c r="C2" s="8" t="s">
         <v>457</v>
       </c>
       <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="19"/>
+      <c r="A3" s="18"/>
       <c r="D3" s="12"/>
     </row>
     <row r="4" spans="1:5" ht="21">
-      <c r="A4" s="19"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -3092,7 +3085,7 @@
       </c>
     </row>
     <row r="87" spans="1:5" ht="21">
-      <c r="A87" s="16">
+      <c r="A87" s="15">
         <v>78</v>
       </c>
       <c r="B87" s="3" t="s">
@@ -3106,7 +3099,7 @@
       </c>
     </row>
     <row r="88" spans="1:5" ht="21">
-      <c r="A88" s="16">
+      <c r="A88" s="15">
         <v>79</v>
       </c>
       <c r="B88" s="3" t="s">
@@ -3120,7 +3113,7 @@
       </c>
     </row>
     <row r="89" spans="1:5" ht="21">
-      <c r="A89" s="16">
+      <c r="A89" s="15">
         <v>80</v>
       </c>
       <c r="B89" s="3" t="s">
@@ -3134,7 +3127,7 @@
       </c>
     </row>
     <row r="90" spans="1:5" ht="21">
-      <c r="A90" s="16">
+      <c r="A90" s="15">
         <v>81</v>
       </c>
       <c r="B90" s="3" t="s">
@@ -3148,7 +3141,7 @@
       </c>
     </row>
     <row r="91" spans="1:5" ht="21">
-      <c r="A91" s="16">
+      <c r="A91" s="15">
         <v>82</v>
       </c>
       <c r="B91" s="3" t="s">
@@ -3160,10 +3153,10 @@
       <c r="D91" s="11" t="s">
         <v>458</v>
       </c>
-      <c r="E91" s="17"/>
+      <c r="E91" s="16"/>
     </row>
     <row r="92" spans="1:5" ht="21">
-      <c r="A92" s="18">
+      <c r="A92" s="17">
         <v>83</v>
       </c>
       <c r="B92" s="3" t="s">
@@ -3175,7 +3168,7 @@
       <c r="D92" s="11" t="s">
         <v>458</v>
       </c>
-      <c r="E92" s="17" t="s">
+      <c r="E92" s="16" t="s">
         <v>470</v>
       </c>
     </row>
@@ -3192,10 +3185,10 @@
       <c r="D93" s="11" t="s">
         <v>458</v>
       </c>
-      <c r="E93" s="17"/>
+      <c r="E93" s="16"/>
     </row>
     <row r="94" spans="1:5" ht="21">
-      <c r="A94">
+      <c r="A94" s="15">
         <v>85</v>
       </c>
       <c r="B94" s="3" t="s">
@@ -3204,10 +3197,10 @@
       <c r="C94" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D94" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E94" s="17"/>
+      <c r="D94" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="E94" s="16"/>
     </row>
     <row r="95" spans="1:5" ht="21">
       <c r="A95">
@@ -3222,7 +3215,7 @@
       <c r="D95" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E95" s="17"/>
+      <c r="E95" s="16"/>
     </row>
     <row r="96" spans="1:5" ht="21">
       <c r="A96">
@@ -3237,7 +3230,7 @@
       <c r="D96" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E96" s="17"/>
+      <c r="E96" s="16"/>
     </row>
     <row r="97" spans="1:5" ht="21">
       <c r="A97">
@@ -3252,7 +3245,7 @@
       <c r="D97" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E97" s="17"/>
+      <c r="E97" s="16"/>
     </row>
     <row r="98" spans="1:5" ht="21">
       <c r="A98">
@@ -3267,7 +3260,7 @@
       <c r="D98" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E98" s="17"/>
+      <c r="E98" s="16"/>
     </row>
     <row r="100" spans="1:5" ht="21">
       <c r="B100" s="6"/>
@@ -3795,7 +3788,7 @@
       <c r="D139" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E139" s="17">
+      <c r="E139" s="16">
         <v>44326</v>
       </c>
     </row>
@@ -3812,7 +3805,7 @@
       <c r="D140" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E140" s="17">
+      <c r="E140" s="16">
         <v>44326</v>
       </c>
     </row>
@@ -3829,7 +3822,7 @@
       <c r="D141" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E141" s="17">
+      <c r="E141" s="16">
         <v>44327</v>
       </c>
     </row>
@@ -3846,7 +3839,7 @@
       <c r="D142" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E142" s="17">
+      <c r="E142" s="16">
         <v>44327</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Transform one string to another added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6178FF2C-61B1-466E-A74F-7806928E3D40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DEB5C9-8A09-45D4-9E64-67E58FD5370E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1933,8 +1933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:E481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3218,7 +3218,7 @@
       <c r="E95" s="16"/>
     </row>
     <row r="96" spans="1:5" ht="21">
-      <c r="A96">
+      <c r="A96" s="15">
         <v>87</v>
       </c>
       <c r="B96" s="3" t="s">
@@ -3227,8 +3227,8 @@
       <c r="C96" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D96" s="10" t="s">
-        <v>4</v>
+      <c r="D96" s="11" t="s">
+        <v>458</v>
       </c>
       <c r="E96" s="16"/>
     </row>

</xml_diff>

<commit_message>
First and last occurence of a number added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B33287-F482-452F-8C01-005FF6126F19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF2BBB7-1FA4-4B05-902A-ECD996124059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="472">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1434,17 +1434,20 @@
     <t>Write a program tofind the smallest window that contains all characters of string itself. (Please see pep coding soln in youtube for clarity)</t>
   </si>
   <si>
-    <t>Date to be completed by</t>
-  </si>
-  <si>
     <t>VERY VERY TOUGH AND MOST IMP … BAAAP of all Sliding Window Question)</t>
+  </si>
+  <si>
+    <t>Didn't get how to do</t>
+  </si>
+  <si>
+    <t>DATE REVISED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1528,8 +1531,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1558,8 +1575,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1567,14 +1594,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1611,13 +1655,19 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Input" xfId="5" builtinId="20"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1933,43 +1983,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:E481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="5.09765625" customWidth="1"/>
     <col min="2" max="2" width="28.5" customWidth="1"/>
     <col min="3" max="3" width="159.8984375" customWidth="1"/>
-    <col min="4" max="4" width="12.5" style="9" customWidth="1"/>
+    <col min="4" max="4" width="23.296875" style="9" customWidth="1"/>
     <col min="5" max="5" width="23.09765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24.6">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>459</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
-        <v>469</v>
+      <c r="E1" s="20" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="18"/>
+      <c r="A2" s="19"/>
       <c r="C2" s="8" t="s">
         <v>457</v>
       </c>
       <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="18"/>
+      <c r="A3" s="19"/>
       <c r="D3" s="12"/>
     </row>
     <row r="4" spans="1:5" ht="21">
-      <c r="A4" s="18"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -2002,6 +2052,9 @@
       <c r="D6" s="11" t="s">
         <v>458</v>
       </c>
+      <c r="E6" s="16">
+        <v>44349</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="21">
       <c r="A7" s="12">
@@ -2015,6 +2068,9 @@
       </c>
       <c r="D7" s="11" t="s">
         <v>458</v>
+      </c>
+      <c r="E7" s="16">
+        <v>44349</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="21">
@@ -3169,7 +3225,7 @@
         <v>458</v>
       </c>
       <c r="E92" s="16" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="21">
@@ -3248,7 +3304,7 @@
       <c r="E97" s="16"/>
     </row>
     <row r="98" spans="1:5" ht="21">
-      <c r="A98">
+      <c r="A98" s="18">
         <v>89</v>
       </c>
       <c r="B98" s="3" t="s">
@@ -3260,7 +3316,9 @@
       <c r="D98" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E98" s="16"/>
+      <c r="E98" s="16" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="100" spans="1:5" ht="21">
       <c r="B100" s="6"/>

</xml_diff>

<commit_message>
First and last occurence optimal sol added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF2BBB7-1FA4-4B05-902A-ECD996124059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38637F27-FC33-4B3E-8CF5-20EB1DBBF5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="473">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1441,6 +1441,9 @@
   </si>
   <si>
     <t>DATE REVISED</t>
+  </si>
+  <si>
+    <t>Easy q… Think next time</t>
   </si>
 </sst>
 </file>
@@ -1656,10 +1659,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="5" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1983,8 +1986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:E481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1997,29 +2000,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24.6">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>459</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="19"/>
+      <c r="A2" s="20"/>
       <c r="C2" s="8" t="s">
         <v>457</v>
       </c>
       <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="19"/>
+      <c r="A3" s="20"/>
       <c r="D3" s="12"/>
     </row>
     <row r="4" spans="1:5" ht="21">
-      <c r="A4" s="19"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -3320,13 +3323,16 @@
         <v>470</v>
       </c>
     </row>
+    <row r="99" spans="1:5">
+      <c r="D99"/>
+    </row>
     <row r="100" spans="1:5" ht="21">
       <c r="B100" s="6"/>
       <c r="C100" s="5"/>
-      <c r="D100" s="10"/>
+      <c r="D100"/>
     </row>
     <row r="101" spans="1:5" ht="21">
-      <c r="A101">
+      <c r="A101" s="15">
         <v>90</v>
       </c>
       <c r="B101" s="3" t="s">
@@ -3335,8 +3341,11 @@
       <c r="C101" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D101" s="10" t="s">
-        <v>4</v>
+      <c r="D101" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="E101" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="21">

</xml_diff>

<commit_message>
Intersection of two arrays added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38637F27-FC33-4B3E-8CF5-20EB1DBBF5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF63AEE-B2D3-4336-9BE7-0CEED4B6A079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1986,8 +1986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:E481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="E101" sqref="E101"/>
+    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2089,6 +2089,9 @@
       <c r="D8" s="11" t="s">
         <v>458</v>
       </c>
+      <c r="E8" s="16">
+        <v>44351</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="21">
       <c r="A9" s="12">
@@ -2119,7 +2122,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="21">
-      <c r="A11" s="12">
+      <c r="A11" s="15">
         <v>6</v>
       </c>
       <c r="B11" s="3" t="s">

</xml_diff>

<commit_message>
Value equal to index value
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF63AEE-B2D3-4336-9BE7-0CEED4B6A079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A199F39-FD20-4B4D-8A17-AB70B8999FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1986,8 +1986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:E481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3352,7 +3352,7 @@
       </c>
     </row>
     <row r="102" spans="1:5" ht="21">
-      <c r="A102">
+      <c r="A102" s="12">
         <v>91</v>
       </c>
       <c r="B102" s="3" t="s">
@@ -3361,8 +3361,8 @@
       <c r="C102" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D102" s="10" t="s">
-        <v>4</v>
+      <c r="D102" s="11" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="21">

</xml_diff>

<commit_message>
Added search in rotated sorted array
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A199F39-FD20-4B4D-8A17-AB70B8999FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95725B6-4662-40CA-BFF5-2A93872551CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="474">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1444,6 +1444,9 @@
   </si>
   <si>
     <t>Easy q… Think next time</t>
+  </si>
+  <si>
+    <t>Did this Medium level difficulty q on my own and received 100% faster soln… I am sooooo happy now</t>
   </si>
 </sst>
 </file>
@@ -1986,8 +1989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:E481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3366,7 +3369,7 @@
       </c>
     </row>
     <row r="103" spans="1:5" ht="21">
-      <c r="A103">
+      <c r="A103" s="12">
         <v>92</v>
       </c>
       <c r="B103" s="3" t="s">
@@ -3375,8 +3378,11 @@
       <c r="C103" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D103" s="10" t="s">
-        <v>4</v>
+      <c r="D103" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="E103" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="21">

</xml_diff>

<commit_message>
Added another code in Pointers
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D0BD12-3D91-4D12-AD8E-4156EC0C9946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343539B4-8DAE-4820-B65C-7D4F01C10B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1989,8 +1989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:E481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView tabSelected="1" topLeftCell="C92" zoomScale="76" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3428,7 +3428,7 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="21">
-      <c r="A107">
+      <c r="A107" s="15">
         <v>96</v>
       </c>
       <c r="B107" s="3" t="s">

</xml_diff>

<commit_message>
Added find missing and repeating's best solution
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8AA123-1CB7-46A0-8CDF-BC279C8BE332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E5BBBB-08F5-49C9-B859-A2934DC4BCF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1989,8 +1989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:E481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="91" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+    <sheetView tabSelected="1" topLeftCell="B42" zoomScale="78" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2108,6 +2108,9 @@
       </c>
       <c r="D9" s="11" t="s">
         <v>458</v>
+      </c>
+      <c r="E9" s="16">
+        <v>44363</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="21">

</xml_diff>

<commit_message>
Added the explanation for problem 09
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5E432F-7413-4D33-8250-CD4921E5CF7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F387D1-31B1-4E9C-A709-9EE48C27EA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1690,12 +1690,12 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="5" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2018,8 +2018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="78" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2032,7 +2032,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24.6">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>459</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -2041,23 +2041,23 @@
       <c r="E1" s="19" t="s">
         <v>472</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>473</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="20"/>
+      <c r="A2" s="22"/>
       <c r="C2" s="8" t="s">
         <v>457</v>
       </c>
       <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="20"/>
+      <c r="A3" s="22"/>
       <c r="D3" s="12"/>
     </row>
     <row r="4" spans="1:6" ht="21">
-      <c r="A4" s="20"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -2164,7 +2164,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="21">
-      <c r="A11" s="15">
+      <c r="A11" s="12">
         <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2175,6 +2175,9 @@
       </c>
       <c r="D11" s="11" t="s">
         <v>458</v>
+      </c>
+      <c r="F11" s="16">
+        <v>44364</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="21">
@@ -2190,6 +2193,9 @@
       <c r="D12" s="11" t="s">
         <v>458</v>
       </c>
+      <c r="F12" s="16">
+        <v>44364</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="21">
       <c r="A13" s="12">
@@ -2204,6 +2210,9 @@
       <c r="D13" s="11" t="s">
         <v>458</v>
       </c>
+      <c r="F13" s="16">
+        <v>44364</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="21">
       <c r="A14" s="15">
@@ -2596,7 +2605,7 @@
       <c r="D41" s="11" t="s">
         <v>458</v>
       </c>
-      <c r="E41" s="22" t="s">
+      <c r="E41" s="21" t="s">
         <v>463</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Find Majority element added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F387D1-31B1-4E9C-A709-9EE48C27EA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABED99B-6D0A-4157-BDA7-57DF569F4403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2018,8 +2018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="78" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2227,6 +2227,9 @@
       <c r="D14" s="11" t="s">
         <v>458</v>
       </c>
+      <c r="F14" s="16">
+        <v>44364</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="21">
       <c r="A15" s="15">
@@ -3471,7 +3474,7 @@
       </c>
     </row>
     <row r="106" spans="1:5" ht="21">
-      <c r="A106">
+      <c r="A106" s="15">
         <v>95</v>
       </c>
       <c r="B106" s="3" t="s">
@@ -3502,7 +3505,7 @@
       </c>
     </row>
     <row r="108" spans="1:5" ht="21">
-      <c r="A108">
+      <c r="A108" s="15">
         <v>97</v>
       </c>
       <c r="B108" s="3" t="s">

</xml_diff>

<commit_message>
Added the Moore's Voting Algo logic
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABED99B-6D0A-4157-BDA7-57DF569F4403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AD24AC-8EF8-407C-AF58-3BC610FACA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="479">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1459,6 +1459,9 @@
   </si>
   <si>
     <t xml:space="preserve">Read Manachers Algo.. See downloaded Video </t>
+  </si>
+  <si>
+    <t>Moore's Voting Algo learnt</t>
   </si>
 </sst>
 </file>
@@ -2018,8 +2021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="78" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="78" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3514,8 +3517,11 @@
       <c r="C108" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D108" s="10" t="s">
-        <v>4</v>
+      <c r="D108" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="E108" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="21">

</xml_diff>

<commit_message>
Made changes in Excel Sheet
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AD24AC-8EF8-407C-AF58-3BC610FACA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD45B25-5066-4EDD-BA5C-6138D48E93EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1461,7 +1461,7 @@
     <t xml:space="preserve">Read Manachers Algo.. See downloaded Video </t>
   </si>
   <si>
-    <t>Moore's Voting Algo learnt</t>
+    <t>Moore's Voting Algo learnt (17-07-21)</t>
   </si>
 </sst>
 </file>
@@ -2021,8 +2021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="78" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="C109" sqref="C109"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="78" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>

</xml_diff>

<commit_message>
Pair with given difference added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD45B25-5066-4EDD-BA5C-6138D48E93EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9492DC58-B52E-453D-98D0-695E67D6CBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="480">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1462,6 +1462,9 @@
   </si>
   <si>
     <t>Moore's Voting Algo learnt (17-07-21)</t>
+  </si>
+  <si>
+    <t>Think about abt the soln next time. It's easy</t>
   </si>
 </sst>
 </file>
@@ -2021,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="78" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="78" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3525,7 +3528,7 @@
       </c>
     </row>
     <row r="109" spans="1:5" ht="21">
-      <c r="A109">
+      <c r="A109" s="15">
         <v>98</v>
       </c>
       <c r="B109" s="3" t="s">
@@ -3534,8 +3537,11 @@
       <c r="C109" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D109" s="10" t="s">
-        <v>4</v>
+      <c r="D109" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="E109" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="21">

</xml_diff>

<commit_message>
Pair with given Pair optimised soln added
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9492DC58-B52E-453D-98D0-695E67D6CBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9334275-DC53-4AB5-82AF-5E2715083151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="481">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1465,6 +1465,9 @@
   </si>
   <si>
     <t>Think about abt the soln next time. It's easy</t>
+  </si>
+  <si>
+    <t>Did by my own. Really Happy</t>
   </si>
 </sst>
 </file>
@@ -2025,7 +2028,7 @@
   <dimension ref="A1:F481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A103" zoomScale="78" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="B110" sqref="B110"/>
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3545,7 +3548,7 @@
       </c>
     </row>
     <row r="110" spans="1:5" ht="21">
-      <c r="A110">
+      <c r="A110" s="12">
         <v>99</v>
       </c>
       <c r="B110" s="3" t="s">
@@ -3554,8 +3557,11 @@
       <c r="C110" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D110" s="10" t="s">
-        <v>4</v>
+      <c r="D110" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="E110" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="21">

</xml_diff>

<commit_message>
Added screenshots and updated excel sheet
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9334275-DC53-4AB5-82AF-5E2715083151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB9640C-7171-4B1B-8315-367E3CD7AECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2027,8 +2027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="78" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="57" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="D111" sqref="D111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3565,7 +3565,7 @@
       </c>
     </row>
     <row r="111" spans="1:5" ht="21">
-      <c r="A111">
+      <c r="A111" s="15">
         <v>100</v>
       </c>
       <c r="B111" s="3" t="s">
@@ -3574,8 +3574,8 @@
       <c r="C111" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D111" s="10" t="s">
-        <v>4</v>
+      <c r="D111" s="11" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="21">

</xml_diff>

<commit_message>
Added more coding problems
</commit_message>
<xml_diff>
--- a/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
+++ b/450 Questions for DSA/FINAL450 Qs for DS ALGo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\450 Questions for DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F3A496-75F5-4CA6-B7C5-791B5A90B9C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2A466F-7A86-4757-AA15-EEEA6436FA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2030,8 +2030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="78" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="78" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>

</xml_diff>